<commit_message>
several bugs in bitstream occurred - configuration bits in VHDL model do not match with PCB - configuration bits in VHDL don't match with excel sheet - set_reg_* bits don't map correctly - LUT bits don't map correctly
let's just redo the entire bitstream documentation.
take PCB as reference, adapt to VHDL, document in excel
</commit_message>
<xml_diff>
--- a/doc/bitstream_doc.xlsx
+++ b/doc/bitstream_doc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Downloads\FPGA\my-discrete-fpga\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5A07C3-8E06-470C-9B13-7127FB76E249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{075103CA-0FDB-4641-B9F9-0DAD6D761FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14400" yWindow="0" windowWidth="14400" windowHeight="16200" xr2:uid="{C7546AD3-8A64-4A61-AF3E-FA211CF4A71C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="24890" windowHeight="14620" xr2:uid="{C7546AD3-8A64-4A61-AF3E-FA211CF4A71C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="157">
   <si>
     <t>Bitstream Documentation for one full slice</t>
   </si>
@@ -386,75 +386,15 @@
     <t>LUT3a1[0]</t>
   </si>
   <si>
-    <t>LUT3a1[7]</t>
-  </si>
-  <si>
-    <t>LUT3a1</t>
-  </si>
-  <si>
     <t>LUT3a0[0]</t>
   </si>
   <si>
-    <t>LUT3a0</t>
-  </si>
-  <si>
-    <t>LUT3a0[7]</t>
-  </si>
-  <si>
-    <t>LUT3d0</t>
-  </si>
-  <si>
-    <t>LUT3d1</t>
-  </si>
-  <si>
-    <t>LUT3 D0</t>
-  </si>
-  <si>
-    <t>LUT3 D1</t>
-  </si>
-  <si>
-    <t>LUT3 C0</t>
-  </si>
-  <si>
-    <t>LUT3 C1</t>
-  </si>
-  <si>
-    <t>LUT3 B0</t>
-  </si>
-  <si>
-    <t>LUT3 B1</t>
-  </si>
-  <si>
-    <t>LUT3 A0</t>
-  </si>
-  <si>
-    <t>LUT3 A1</t>
-  </si>
-  <si>
-    <t>LUT3b1</t>
-  </si>
-  <si>
-    <t>LUT3b0</t>
-  </si>
-  <si>
-    <t>LUT3c1</t>
-  </si>
-  <si>
-    <t>LUT3c0</t>
-  </si>
-  <si>
     <t>LUT3d1[0]</t>
   </si>
   <si>
-    <t>LUT3d1[7]</t>
-  </si>
-  <si>
     <t>LUT3d0[0]</t>
   </si>
   <si>
-    <t>LUT3d0[7]</t>
-  </si>
-  <si>
     <t>LUT3c0[0]</t>
   </si>
   <si>
@@ -467,18 +407,6 @@
     <t>LUT3b1[0]</t>
   </si>
   <si>
-    <t>LUT3b1[7]</t>
-  </si>
-  <si>
-    <t>LUT3b0[7]</t>
-  </si>
-  <si>
-    <t>LUT3c1[7]</t>
-  </si>
-  <si>
-    <t>LUT3c0[7]</t>
-  </si>
-  <si>
     <t>sel_0[0]</t>
   </si>
   <si>
@@ -567,6 +495,18 @@
   </si>
   <si>
     <t>presel_2[2]</t>
+  </si>
+  <si>
+    <t>LUT C</t>
+  </si>
+  <si>
+    <t>LUT B</t>
+  </si>
+  <si>
+    <t>LUT A</t>
+  </si>
+  <si>
+    <t>LUT D</t>
   </si>
 </sst>
 </file>
@@ -941,24 +881,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B05D7D6F-9919-4953-A5D7-1B3682A8C1CB}">
   <dimension ref="A1:H143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="B140" sqref="B140:G143"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="L74" sqref="L74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="5" width="9.140625" style="2"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" customWidth="1"/>
-    <col min="8" max="8" width="59.5703125" style="3" customWidth="1"/>
+    <col min="4" max="5" width="9.1796875" style="2"/>
+    <col min="6" max="6" width="14.54296875" customWidth="1"/>
+    <col min="7" max="7" width="22.26953125" customWidth="1"/>
+    <col min="8" max="8" width="59.54296875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>1</v>
       </c>
@@ -978,7 +918,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B8" s="4">
         <v>0</v>
       </c>
@@ -998,7 +938,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B9" s="4">
         <v>1</v>
       </c>
@@ -1015,7 +955,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B10" s="4">
         <v>2</v>
       </c>
@@ -1032,7 +972,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B11" s="4">
         <v>3</v>
       </c>
@@ -1049,7 +989,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B12" s="4">
         <v>4</v>
       </c>
@@ -1066,7 +1006,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B13" s="4">
         <v>5</v>
       </c>
@@ -1083,7 +1023,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B14" s="4">
         <v>6</v>
       </c>
@@ -1100,7 +1040,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B15" s="4">
         <v>7</v>
       </c>
@@ -1120,7 +1060,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B16" s="4">
         <v>8</v>
       </c>
@@ -1130,11 +1070,8 @@
       <c r="E16" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F16" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B17" s="4">
         <v>9</v>
       </c>
@@ -1144,11 +1081,8 @@
       <c r="E17" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F17" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B18" s="4">
         <v>10</v>
       </c>
@@ -1158,11 +1092,8 @@
       <c r="E18" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B19" s="4">
         <v>11</v>
       </c>
@@ -1172,11 +1103,8 @@
       <c r="E19" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F19" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B20" s="4">
         <v>12</v>
       </c>
@@ -1186,11 +1114,8 @@
       <c r="E20" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F20" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B21" s="4">
         <v>13</v>
       </c>
@@ -1200,11 +1125,8 @@
       <c r="E21" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F21" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B22" s="4">
         <v>14</v>
       </c>
@@ -1214,11 +1136,8 @@
       <c r="E22" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F22" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B23" s="4">
         <v>15</v>
       </c>
@@ -1229,13 +1148,13 @@
         <v>87</v>
       </c>
       <c r="F23" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="G23" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B24" s="4">
         <v>16</v>
       </c>
@@ -1245,11 +1164,8 @@
       <c r="E24" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F24" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B25" s="4">
         <v>17</v>
       </c>
@@ -1259,11 +1175,8 @@
       <c r="E25" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F25" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B26" s="4">
         <v>18</v>
       </c>
@@ -1273,11 +1186,8 @@
       <c r="E26" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F26" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B27" s="4">
         <v>19</v>
       </c>
@@ -1287,11 +1197,8 @@
       <c r="E27" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F27" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B28" s="4">
         <v>20</v>
       </c>
@@ -1301,11 +1208,8 @@
       <c r="E28" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F28" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B29" s="4">
         <v>21</v>
       </c>
@@ -1315,11 +1219,8 @@
       <c r="E29" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F29" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B30" s="4">
         <v>22</v>
       </c>
@@ -1329,11 +1230,8 @@
       <c r="E30" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F30" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B31" s="4">
         <v>23</v>
       </c>
@@ -1344,13 +1242,13 @@
         <v>87</v>
       </c>
       <c r="F31" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="G31" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B32" s="4">
         <v>24</v>
       </c>
@@ -1360,11 +1258,8 @@
       <c r="E32" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F32" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B33" s="4">
         <v>25</v>
       </c>
@@ -1374,11 +1269,8 @@
       <c r="E33" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F33" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B34" s="4">
         <v>26</v>
       </c>
@@ -1388,11 +1280,8 @@
       <c r="E34" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F34" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B35" s="4">
         <v>27</v>
       </c>
@@ -1402,11 +1291,8 @@
       <c r="E35" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F35" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B36" s="4">
         <v>28</v>
       </c>
@@ -1416,11 +1302,8 @@
       <c r="E36" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F36" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B37" s="4">
         <v>29</v>
       </c>
@@ -1430,11 +1313,8 @@
       <c r="E37" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F37" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B38" s="4">
         <v>30</v>
       </c>
@@ -1444,11 +1324,8 @@
       <c r="E38" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F38" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B39" s="4">
         <v>31</v>
       </c>
@@ -1459,13 +1336,13 @@
         <v>87</v>
       </c>
       <c r="F39" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
       <c r="G39" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B40" s="4">
         <v>32</v>
       </c>
@@ -1475,11 +1352,8 @@
       <c r="E40" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F40" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B41" s="4">
         <v>33</v>
       </c>
@@ -1489,11 +1363,8 @@
       <c r="E41" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F41" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B42" s="4">
         <v>34</v>
       </c>
@@ -1503,11 +1374,8 @@
       <c r="E42" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F42" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B43" s="4">
         <v>35</v>
       </c>
@@ -1517,11 +1385,8 @@
       <c r="E43" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F43" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B44" s="4">
         <v>36</v>
       </c>
@@ -1531,11 +1396,8 @@
       <c r="E44" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F44" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B45" s="4">
         <v>37</v>
       </c>
@@ -1545,11 +1407,8 @@
       <c r="E45" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F45" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B46" s="4">
         <v>38</v>
       </c>
@@ -1559,11 +1418,8 @@
       <c r="E46" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F46" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B47" s="4">
         <v>39</v>
       </c>
@@ -1574,13 +1430,13 @@
         <v>87</v>
       </c>
       <c r="F47" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="G47" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B48" s="4">
         <v>40</v>
       </c>
@@ -1590,11 +1446,8 @@
       <c r="E48" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F48" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B49" s="4">
         <v>41</v>
       </c>
@@ -1604,11 +1457,8 @@
       <c r="E49" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F49" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B50" s="4">
         <v>42</v>
       </c>
@@ -1618,11 +1468,8 @@
       <c r="E50" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F50" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B51" s="4">
         <v>43</v>
       </c>
@@ -1632,11 +1479,8 @@
       <c r="E51" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F51" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B52" s="4">
         <v>44</v>
       </c>
@@ -1646,11 +1490,8 @@
       <c r="E52" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F52" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B53" s="4">
         <v>45</v>
       </c>
@@ -1660,11 +1501,8 @@
       <c r="E53" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F53" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B54" s="4">
         <v>46</v>
       </c>
@@ -1674,11 +1512,8 @@
       <c r="E54" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F54" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B55" s="4">
         <v>47</v>
       </c>
@@ -1689,13 +1524,13 @@
         <v>87</v>
       </c>
       <c r="F55" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="G55" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B56" s="4">
         <v>48</v>
       </c>
@@ -1705,11 +1540,8 @@
       <c r="E56" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F56" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B57" s="4">
         <v>49</v>
       </c>
@@ -1719,11 +1551,8 @@
       <c r="E57" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F57" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B58" s="4">
         <v>50</v>
       </c>
@@ -1733,11 +1562,8 @@
       <c r="E58" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F58" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B59" s="4">
         <v>51</v>
       </c>
@@ -1747,11 +1573,8 @@
       <c r="E59" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F59" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B60" s="4">
         <v>52</v>
       </c>
@@ -1761,11 +1584,8 @@
       <c r="E60" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F60" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B61" s="4">
         <v>53</v>
       </c>
@@ -1775,11 +1595,8 @@
       <c r="E61" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F61" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B62" s="4">
         <v>54</v>
       </c>
@@ -1789,11 +1606,8 @@
       <c r="E62" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F62" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B63" s="4">
         <v>55</v>
       </c>
@@ -1804,13 +1618,13 @@
         <v>87</v>
       </c>
       <c r="F63" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="G63" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B64" s="4">
         <v>56</v>
       </c>
@@ -1820,11 +1634,8 @@
       <c r="E64" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F64" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B65" s="4">
         <v>57</v>
       </c>
@@ -1834,11 +1645,8 @@
       <c r="E65" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F65" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B66" s="4">
         <v>58</v>
       </c>
@@ -1848,11 +1656,8 @@
       <c r="E66" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F66" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B67" s="4">
         <v>59</v>
       </c>
@@ -1862,11 +1667,8 @@
       <c r="E67" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F67" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B68" s="4">
         <v>60</v>
       </c>
@@ -1876,11 +1678,8 @@
       <c r="E68" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F68" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B69" s="4">
         <v>61</v>
       </c>
@@ -1890,11 +1689,8 @@
       <c r="E69" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F69" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B70" s="4">
         <v>62</v>
       </c>
@@ -1904,11 +1700,8 @@
       <c r="E70" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F70" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B71" s="4">
         <v>63</v>
       </c>
@@ -1919,13 +1712,13 @@
         <v>87</v>
       </c>
       <c r="F71" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G71" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B72" s="4">
         <v>64</v>
       </c>
@@ -1935,11 +1728,8 @@
       <c r="E72" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F72" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B73" s="4">
         <v>65</v>
       </c>
@@ -1949,11 +1739,8 @@
       <c r="E73" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F73" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B74" s="4">
         <v>66</v>
       </c>
@@ -1963,11 +1750,8 @@
       <c r="E74" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F74" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B75" s="4">
         <v>67</v>
       </c>
@@ -1977,11 +1761,8 @@
       <c r="E75" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F75" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B76" s="4">
         <v>68</v>
       </c>
@@ -1991,11 +1772,8 @@
       <c r="E76" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F76" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B77" s="4">
         <v>69</v>
       </c>
@@ -2005,11 +1783,8 @@
       <c r="E77" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F77" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B78" s="4">
         <v>70</v>
       </c>
@@ -2019,11 +1794,8 @@
       <c r="E78" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F78" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B79" s="4">
         <v>71</v>
       </c>
@@ -2037,10 +1809,10 @@
         <v>115</v>
       </c>
       <c r="G79" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B80" s="4">
         <v>72</v>
       </c>
@@ -2057,7 +1829,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B81" s="4">
         <v>73</v>
       </c>
@@ -2074,7 +1846,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B82" s="4">
         <v>74</v>
       </c>
@@ -2091,7 +1863,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B83" s="4">
         <v>75</v>
       </c>
@@ -2108,7 +1880,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B84" s="4">
         <v>76</v>
       </c>
@@ -2125,7 +1897,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B85" s="4">
         <v>77</v>
       </c>
@@ -2142,7 +1914,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B86" s="4">
         <v>78</v>
       </c>
@@ -2159,7 +1931,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B87" s="4">
         <v>79</v>
       </c>
@@ -2176,7 +1948,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B88" s="4">
         <v>80</v>
       </c>
@@ -2193,7 +1965,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B89" s="4">
         <v>81</v>
       </c>
@@ -2210,7 +1982,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B90" s="4">
         <v>82</v>
       </c>
@@ -2227,7 +1999,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B91" s="4">
         <v>83</v>
       </c>
@@ -2244,7 +2016,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B92" s="4">
         <v>84</v>
       </c>
@@ -2261,7 +2033,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B93" s="4">
         <v>85</v>
       </c>
@@ -2278,7 +2050,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B94" s="4">
         <v>86</v>
       </c>
@@ -2295,7 +2067,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B95" s="4">
         <v>87</v>
       </c>
@@ -2312,7 +2084,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B96" s="4">
         <v>88</v>
       </c>
@@ -2329,7 +2101,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B97" s="4">
         <v>89</v>
       </c>
@@ -2340,13 +2112,13 @@
         <v>68</v>
       </c>
       <c r="F97" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="G97" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B98" s="4">
         <v>90</v>
       </c>
@@ -2357,13 +2129,13 @@
         <v>68</v>
       </c>
       <c r="F98" t="s">
-        <v>158</v>
+        <v>134</v>
       </c>
       <c r="G98" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="99" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B99" s="4">
         <v>91</v>
       </c>
@@ -2374,13 +2146,13 @@
         <v>68</v>
       </c>
       <c r="F99" t="s">
-        <v>157</v>
+        <v>133</v>
       </c>
       <c r="G99" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="100" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B100" s="4">
         <v>92</v>
       </c>
@@ -2391,16 +2163,16 @@
         <v>68</v>
       </c>
       <c r="F100" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="G100" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="H100" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="101" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B101" s="4">
         <v>93</v>
       </c>
@@ -2411,13 +2183,13 @@
         <v>68</v>
       </c>
       <c r="F101" t="s">
-        <v>149</v>
+        <v>125</v>
       </c>
       <c r="G101" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="102" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B102" s="4">
         <v>94</v>
       </c>
@@ -2428,13 +2200,13 @@
         <v>68</v>
       </c>
       <c r="F102" t="s">
-        <v>156</v>
+        <v>132</v>
       </c>
       <c r="G102" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="103" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B103" s="4">
         <v>95</v>
       </c>
@@ -2445,13 +2217,13 @@
         <v>68</v>
       </c>
       <c r="F103" t="s">
-        <v>155</v>
+        <v>131</v>
       </c>
       <c r="G103" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="104" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B104" s="4">
         <v>96</v>
       </c>
@@ -2462,16 +2234,16 @@
         <v>68</v>
       </c>
       <c r="F104" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="G104" t="s">
-        <v>164</v>
+        <v>140</v>
       </c>
       <c r="H104" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="105" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B105" s="4">
         <v>97</v>
       </c>
@@ -2482,13 +2254,13 @@
         <v>68</v>
       </c>
       <c r="F105" t="s">
-        <v>154</v>
+        <v>130</v>
       </c>
       <c r="G105" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="106" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B106" s="4">
         <v>98</v>
       </c>
@@ -2499,13 +2271,13 @@
         <v>68</v>
       </c>
       <c r="F106" t="s">
+        <v>124</v>
+      </c>
+      <c r="G106" t="s">
         <v>148</v>
       </c>
-      <c r="G106" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="107" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B107" s="4">
         <v>99</v>
       </c>
@@ -2516,13 +2288,13 @@
         <v>68</v>
       </c>
       <c r="F107" t="s">
-        <v>153</v>
+        <v>129</v>
       </c>
       <c r="G107" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="108" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B108" s="4">
         <v>100</v>
       </c>
@@ -2533,16 +2305,16 @@
         <v>68</v>
       </c>
       <c r="F108" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="G108" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="H108" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="109" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B109" s="4">
         <v>101</v>
       </c>
@@ -2553,13 +2325,13 @@
         <v>68</v>
       </c>
       <c r="F109" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
       <c r="G109" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="110" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B110" s="4">
         <v>102</v>
       </c>
@@ -2570,13 +2342,13 @@
         <v>68</v>
       </c>
       <c r="F110" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="G110" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="111" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B111" s="4">
         <v>103</v>
       </c>
@@ -2587,13 +2359,13 @@
         <v>68</v>
       </c>
       <c r="F111" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="G111" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="112" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B112" s="4">
         <v>104</v>
       </c>
@@ -2610,7 +2382,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B113" s="4">
         <v>105</v>
       </c>
@@ -2627,7 +2399,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B114" s="4">
         <v>106</v>
       </c>
@@ -2644,7 +2416,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B115" s="4">
         <v>107</v>
       </c>
@@ -2661,7 +2433,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B116" s="4">
         <v>108</v>
       </c>
@@ -2678,7 +2450,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="117" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B117" s="4">
         <v>109</v>
       </c>
@@ -2695,7 +2467,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B118" s="4">
         <v>110</v>
       </c>
@@ -2712,7 +2484,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B119" s="4">
         <v>111</v>
       </c>
@@ -2729,7 +2501,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B120" s="4">
         <v>112</v>
       </c>
@@ -2746,7 +2518,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B121" s="4">
         <v>113</v>
       </c>
@@ -2763,7 +2535,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B122" s="4">
         <v>114</v>
       </c>
@@ -2780,7 +2552,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="123" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B123" s="4">
         <v>115</v>
       </c>
@@ -2797,7 +2569,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B124" s="4">
         <v>116</v>
       </c>
@@ -2814,7 +2586,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B125" s="4">
         <v>117</v>
       </c>
@@ -2831,7 +2603,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="126" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B126" s="4">
         <v>118</v>
       </c>
@@ -2848,7 +2620,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="127" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B127" s="4">
         <v>119</v>
       </c>
@@ -2865,7 +2637,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="128" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B128" s="4">
         <v>120</v>
       </c>
@@ -2882,7 +2654,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="129" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B129" s="4">
         <v>121</v>
       </c>
@@ -2899,7 +2671,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="130" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B130" s="4">
         <v>122</v>
       </c>
@@ -2916,7 +2688,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="131" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B131" s="4">
         <v>123</v>
       </c>
@@ -2933,7 +2705,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="132" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B132" s="4">
         <v>124</v>
       </c>
@@ -2950,7 +2722,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="133" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B133" s="4">
         <v>125</v>
       </c>
@@ -2967,7 +2739,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="134" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B134" s="4">
         <v>126</v>
       </c>
@@ -2984,7 +2756,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="135" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B135" s="4">
         <v>127</v>
       </c>
@@ -3001,7 +2773,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="136" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B136" s="4">
         <v>128</v>
       </c>
@@ -3018,7 +2790,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="137" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B137" s="4">
         <v>129</v>
       </c>
@@ -3035,7 +2807,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="138" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B138" s="4">
         <v>130</v>
       </c>
@@ -3052,7 +2824,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="139" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B139" s="4">
         <v>131</v>
       </c>
@@ -3069,7 +2841,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="140" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B140" s="4">
         <v>132</v>
       </c>
@@ -3086,7 +2858,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="141" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B141" s="4">
         <v>133</v>
       </c>
@@ -3103,7 +2875,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="142" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B142" s="4">
         <v>134</v>
       </c>
@@ -3120,7 +2892,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="143" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B143" s="4">
         <v>135</v>
       </c>

</xml_diff>

<commit_message>
IT WORKS! first successful bit toggle simulation using all 4 tile elements - fixed bitstream order issue - fixed delta loop problem - simulation is ready for bitstreams
</commit_message>
<xml_diff>
--- a/doc/bitstream_doc.xlsx
+++ b/doc/bitstream_doc.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Downloads\FPGA\my-discrete-fpga\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{075103CA-0FDB-4641-B9F9-0DAD6D761FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602D1C44-48BD-4D6E-BE5A-80001776F7AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="24890" windowHeight="14620" xr2:uid="{C7546AD3-8A64-4A61-AF3E-FA211CF4A71C}"/>
+    <workbookView xWindow="-28800" yWindow="0" windowWidth="13935" windowHeight="16200" xr2:uid="{C7546AD3-8A64-4A61-AF3E-FA211CF4A71C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="bitstream" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="153">
   <si>
     <t>Bitstream Documentation for one full slice</t>
   </si>
@@ -383,30 +383,6 @@
     <t>&lt;reserved&gt;</t>
   </si>
   <si>
-    <t>LUT3a1[0]</t>
-  </si>
-  <si>
-    <t>LUT3a0[0]</t>
-  </si>
-  <si>
-    <t>LUT3d1[0]</t>
-  </si>
-  <si>
-    <t>LUT3d0[0]</t>
-  </si>
-  <si>
-    <t>LUT3c0[0]</t>
-  </si>
-  <si>
-    <t>LUT3c1[0]</t>
-  </si>
-  <si>
-    <t>LUT3b0[0]</t>
-  </si>
-  <si>
-    <t>LUT3b1[0]</t>
-  </si>
-  <si>
     <t>sel_0[0]</t>
   </si>
   <si>
@@ -497,23 +473,35 @@
     <t>presel_2[2]</t>
   </si>
   <si>
-    <t>LUT C</t>
-  </si>
-  <si>
-    <t>LUT B</t>
-  </si>
-  <si>
-    <t>LUT A</t>
-  </si>
-  <si>
-    <t>LUT D</t>
+    <t>LUT D0</t>
+  </si>
+  <si>
+    <t>LUT D1</t>
+  </si>
+  <si>
+    <t>LUT C0</t>
+  </si>
+  <si>
+    <t>LUT C1</t>
+  </si>
+  <si>
+    <t>LUT B0</t>
+  </si>
+  <si>
+    <t>LUT B1</t>
+  </si>
+  <si>
+    <t>LUT A0</t>
+  </si>
+  <si>
+    <t>LUT A1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -522,25 +510,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -555,7 +549,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -564,7 +558,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -878,27 +873,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B05D7D6F-9919-4953-A5D7-1B3682A8C1CB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC18F46-B9E9-4D36-8A8B-C506C3DCD618}">
   <dimension ref="A1:H143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="L74" sqref="L74"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="5" width="9.1796875" style="2"/>
-    <col min="6" max="6" width="14.54296875" customWidth="1"/>
-    <col min="7" max="7" width="22.26953125" customWidth="1"/>
-    <col min="8" max="8" width="59.54296875" style="3" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="2"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" customWidth="1"/>
+    <col min="8" max="8" width="59.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>1</v>
       </c>
@@ -918,8 +913,8 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B8" s="4">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="5">
         <v>0</v>
       </c>
       <c r="C8">
@@ -938,8 +933,8 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B9" s="4">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="5">
         <v>1</v>
       </c>
       <c r="C9">
@@ -955,8 +950,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B10" s="4">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="5">
         <v>2</v>
       </c>
       <c r="C10">
@@ -972,8 +967,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B11" s="4">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="5">
         <v>3</v>
       </c>
       <c r="C11">
@@ -989,8 +984,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B12" s="4">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="5">
         <v>4</v>
       </c>
       <c r="C12">
@@ -1006,8 +1001,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B13" s="4">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="5">
         <v>5</v>
       </c>
       <c r="C13">
@@ -1023,8 +1018,8 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B14" s="4">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="5">
         <v>6</v>
       </c>
       <c r="C14">
@@ -1040,8 +1035,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B15" s="4">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="5">
         <v>7</v>
       </c>
       <c r="C15">
@@ -1060,8 +1055,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B16" s="4">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="5">
         <v>8</v>
       </c>
       <c r="C16">
@@ -1070,9 +1065,15 @@
       <c r="E16" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B17" s="4">
+      <c r="F16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="5">
         <v>9</v>
       </c>
       <c r="C17">
@@ -1081,9 +1082,15 @@
       <c r="E17" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B18" s="4">
+      <c r="F17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="5">
         <v>10</v>
       </c>
       <c r="C18">
@@ -1092,9 +1099,15 @@
       <c r="E18" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B19" s="4">
+      <c r="F18" t="s">
+        <v>112</v>
+      </c>
+      <c r="G18" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="5">
         <v>11</v>
       </c>
       <c r="C19">
@@ -1103,9 +1116,15 @@
       <c r="E19" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B20" s="4">
+      <c r="F19" t="s">
+        <v>110</v>
+      </c>
+      <c r="G19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="5">
         <v>12</v>
       </c>
       <c r="C20">
@@ -1114,9 +1133,15 @@
       <c r="E20" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B21" s="4">
+      <c r="F20" t="s">
+        <v>101</v>
+      </c>
+      <c r="G20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="5">
         <v>13</v>
       </c>
       <c r="C21">
@@ -1125,9 +1150,15 @@
       <c r="E21" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B22" s="4">
+      <c r="F21" t="s">
+        <v>100</v>
+      </c>
+      <c r="G21" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="5">
         <v>14</v>
       </c>
       <c r="C22">
@@ -1136,9 +1167,15 @@
       <c r="E22" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B23" s="4">
+      <c r="F22" t="s">
+        <v>99</v>
+      </c>
+      <c r="G22" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="5">
         <v>15</v>
       </c>
       <c r="C23">
@@ -1148,14 +1185,14 @@
         <v>87</v>
       </c>
       <c r="F23" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="G23" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B24" s="4">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="5">
         <v>16</v>
       </c>
       <c r="C24">
@@ -1165,8 +1202,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B25" s="4">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="5">
         <v>17</v>
       </c>
       <c r="C25">
@@ -1176,8 +1213,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B26" s="4">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="5">
         <v>18</v>
       </c>
       <c r="C26">
@@ -1187,8 +1224,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B27" s="4">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="5">
         <v>19</v>
       </c>
       <c r="C27">
@@ -1198,8 +1235,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B28" s="4">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="5">
         <v>20</v>
       </c>
       <c r="C28">
@@ -1209,8 +1246,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B29" s="4">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="5">
         <v>21</v>
       </c>
       <c r="C29">
@@ -1220,8 +1257,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B30" s="4">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="5">
         <v>22</v>
       </c>
       <c r="C30">
@@ -1231,8 +1268,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B31" s="4">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="5">
         <v>23</v>
       </c>
       <c r="C31">
@@ -1241,15 +1278,12 @@
       <c r="E31" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F31" t="s">
-        <v>117</v>
-      </c>
       <c r="G31" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B32" s="4">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="5">
         <v>24</v>
       </c>
       <c r="C32">
@@ -1259,8 +1293,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B33" s="4">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="5">
         <v>25</v>
       </c>
       <c r="C33">
@@ -1270,8 +1304,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B34" s="4">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="5">
         <v>26</v>
       </c>
       <c r="C34">
@@ -1281,8 +1315,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B35" s="4">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="5">
         <v>27</v>
       </c>
       <c r="C35">
@@ -1292,8 +1326,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B36" s="4">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="5">
         <v>28</v>
       </c>
       <c r="C36">
@@ -1303,8 +1337,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B37" s="4">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="5">
         <v>29</v>
       </c>
       <c r="C37">
@@ -1314,8 +1348,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B38" s="4">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="5">
         <v>30</v>
       </c>
       <c r="C38">
@@ -1325,8 +1359,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B39" s="4">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="5">
         <v>31</v>
       </c>
       <c r="C39">
@@ -1335,15 +1369,12 @@
       <c r="E39" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F39" t="s">
-        <v>119</v>
-      </c>
       <c r="G39" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B40" s="4">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="5">
         <v>32</v>
       </c>
       <c r="C40">
@@ -1353,8 +1384,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B41" s="4">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="5">
         <v>33</v>
       </c>
       <c r="C41">
@@ -1364,8 +1395,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B42" s="4">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="5">
         <v>34</v>
       </c>
       <c r="C42">
@@ -1375,8 +1406,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B43" s="4">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="5">
         <v>35</v>
       </c>
       <c r="C43">
@@ -1386,8 +1417,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B44" s="4">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="5">
         <v>36</v>
       </c>
       <c r="C44">
@@ -1397,8 +1428,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B45" s="4">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" s="5">
         <v>37</v>
       </c>
       <c r="C45">
@@ -1408,8 +1439,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B46" s="4">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46" s="5">
         <v>38</v>
       </c>
       <c r="C46">
@@ -1419,8 +1450,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B47" s="4">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" s="5">
         <v>39</v>
       </c>
       <c r="C47">
@@ -1429,15 +1460,12 @@
       <c r="E47" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F47" t="s">
-        <v>120</v>
-      </c>
       <c r="G47" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B48" s="4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48" s="5">
         <v>40</v>
       </c>
       <c r="C48">
@@ -1447,8 +1475,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B49" s="4">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="5">
         <v>41</v>
       </c>
       <c r="C49">
@@ -1458,8 +1486,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B50" s="4">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="5">
         <v>42</v>
       </c>
       <c r="C50">
@@ -1469,8 +1497,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B51" s="4">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B51" s="5">
         <v>43</v>
       </c>
       <c r="C51">
@@ -1480,8 +1508,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B52" s="4">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B52" s="5">
         <v>44</v>
       </c>
       <c r="C52">
@@ -1491,8 +1519,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B53" s="4">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B53" s="5">
         <v>45</v>
       </c>
       <c r="C53">
@@ -1502,8 +1530,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B54" s="4">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B54" s="5">
         <v>46</v>
       </c>
       <c r="C54">
@@ -1513,8 +1541,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B55" s="4">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B55" s="5">
         <v>47</v>
       </c>
       <c r="C55">
@@ -1523,15 +1551,12 @@
       <c r="E55" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F55" t="s">
-        <v>121</v>
-      </c>
       <c r="G55" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B56" s="4">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B56" s="5">
         <v>48</v>
       </c>
       <c r="C56">
@@ -1541,8 +1566,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B57" s="4">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B57" s="5">
         <v>49</v>
       </c>
       <c r="C57">
@@ -1552,8 +1577,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B58" s="4">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B58" s="5">
         <v>50</v>
       </c>
       <c r="C58">
@@ -1563,8 +1588,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B59" s="4">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B59" s="5">
         <v>51</v>
       </c>
       <c r="C59">
@@ -1574,8 +1599,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B60" s="4">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B60" s="5">
         <v>52</v>
       </c>
       <c r="C60">
@@ -1585,8 +1610,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B61" s="4">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B61" s="5">
         <v>53</v>
       </c>
       <c r="C61">
@@ -1596,8 +1621,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B62" s="4">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B62" s="5">
         <v>54</v>
       </c>
       <c r="C62">
@@ -1607,8 +1632,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B63" s="4">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B63" s="5">
         <v>55</v>
       </c>
       <c r="C63">
@@ -1617,15 +1642,12 @@
       <c r="E63" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F63" t="s">
-        <v>122</v>
-      </c>
       <c r="G63" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B64" s="4">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B64" s="5">
         <v>56</v>
       </c>
       <c r="C64">
@@ -1635,8 +1657,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B65" s="4">
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B65" s="5">
         <v>57</v>
       </c>
       <c r="C65">
@@ -1646,8 +1668,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B66" s="4">
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B66" s="5">
         <v>58</v>
       </c>
       <c r="C66">
@@ -1657,8 +1679,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B67" s="4">
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B67" s="5">
         <v>59</v>
       </c>
       <c r="C67">
@@ -1668,8 +1690,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B68" s="4">
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B68" s="5">
         <v>60</v>
       </c>
       <c r="C68">
@@ -1679,8 +1701,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B69" s="4">
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B69" s="5">
         <v>61</v>
       </c>
       <c r="C69">
@@ -1690,8 +1712,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B70" s="4">
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B70" s="5">
         <v>62</v>
       </c>
       <c r="C70">
@@ -1701,8 +1723,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B71" s="4">
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B71" s="5">
         <v>63</v>
       </c>
       <c r="C71">
@@ -1711,15 +1733,12 @@
       <c r="E71" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F71" t="s">
-        <v>116</v>
-      </c>
       <c r="G71" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B72" s="4">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B72" s="5">
         <v>64</v>
       </c>
       <c r="C72">
@@ -1729,8 +1748,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B73" s="4">
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B73" s="5">
         <v>65</v>
       </c>
       <c r="C73">
@@ -1740,8 +1759,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B74" s="4">
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B74" s="5">
         <v>66</v>
       </c>
       <c r="C74">
@@ -1751,8 +1770,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B75" s="4">
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B75" s="5">
         <v>67</v>
       </c>
       <c r="C75">
@@ -1762,8 +1781,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B76" s="4">
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B76" s="5">
         <v>68</v>
       </c>
       <c r="C76">
@@ -1773,8 +1792,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B77" s="4">
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B77" s="5">
         <v>69</v>
       </c>
       <c r="C77">
@@ -1784,8 +1803,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B78" s="4">
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B78" s="5">
         <v>70</v>
       </c>
       <c r="C78">
@@ -1795,8 +1814,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B79" s="4">
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B79" s="5">
         <v>71</v>
       </c>
       <c r="C79">
@@ -1805,15 +1824,12 @@
       <c r="E79" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F79" t="s">
-        <v>115</v>
-      </c>
       <c r="G79" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B80" s="4">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B80" s="5">
         <v>72</v>
       </c>
       <c r="C80">
@@ -1822,15 +1838,9 @@
       <c r="E80" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F80" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G80" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B81" s="4">
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B81" s="5">
         <v>73</v>
       </c>
       <c r="C81">
@@ -1839,15 +1849,9 @@
       <c r="E81" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F81" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G81" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B82" s="4">
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B82" s="5">
         <v>74</v>
       </c>
       <c r="C82">
@@ -1856,15 +1860,9 @@
       <c r="E82" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F82" t="s">
-        <v>112</v>
-      </c>
-      <c r="G82" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B83" s="4">
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B83" s="5">
         <v>75</v>
       </c>
       <c r="C83">
@@ -1873,15 +1871,9 @@
       <c r="E83" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F83" t="s">
-        <v>110</v>
-      </c>
-      <c r="G83" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B84" s="4">
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B84" s="5">
         <v>76</v>
       </c>
       <c r="C84">
@@ -1890,15 +1882,9 @@
       <c r="E84" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F84" t="s">
-        <v>101</v>
-      </c>
-      <c r="G84" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B85" s="4">
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B85" s="5">
         <v>77</v>
       </c>
       <c r="C85">
@@ -1907,15 +1893,9 @@
       <c r="E85" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F85" t="s">
-        <v>100</v>
-      </c>
-      <c r="G85" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B86" s="4">
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B86" s="5">
         <v>78</v>
       </c>
       <c r="C86">
@@ -1924,15 +1904,9 @@
       <c r="E86" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F86" t="s">
-        <v>99</v>
-      </c>
-      <c r="G86" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B87" s="4">
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B87" s="5">
         <v>79</v>
       </c>
       <c r="C87">
@@ -1941,15 +1915,12 @@
       <c r="E87" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F87" t="s">
-        <v>98</v>
-      </c>
       <c r="G87" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B88" s="4">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B88" s="5">
         <v>80</v>
       </c>
       <c r="C88">
@@ -1965,8 +1936,8 @@
         <v>105</v>
       </c>
     </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B89" s="4">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B89" s="5">
         <v>81</v>
       </c>
       <c r="C89">
@@ -1982,8 +1953,8 @@
         <v>105</v>
       </c>
     </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B90" s="4">
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B90" s="5">
         <v>82</v>
       </c>
       <c r="C90">
@@ -1999,8 +1970,8 @@
         <v>104</v>
       </c>
     </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B91" s="4">
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B91" s="5">
         <v>83</v>
       </c>
       <c r="C91">
@@ -2016,8 +1987,8 @@
         <v>104</v>
       </c>
     </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B92" s="4">
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B92" s="5">
         <v>84</v>
       </c>
       <c r="C92">
@@ -2033,8 +2004,8 @@
         <v>103</v>
       </c>
     </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B93" s="4">
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B93" s="5">
         <v>85</v>
       </c>
       <c r="C93">
@@ -2050,8 +2021,8 @@
         <v>103</v>
       </c>
     </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B94" s="4">
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B94" s="5">
         <v>86</v>
       </c>
       <c r="C94">
@@ -2067,8 +2038,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B95" s="4">
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B95" s="5">
         <v>87</v>
       </c>
       <c r="C95">
@@ -2084,8 +2055,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B96" s="4">
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B96" s="5">
         <v>88</v>
       </c>
       <c r="C96" s="2">
@@ -2101,8 +2072,8 @@
         <v>114</v>
       </c>
     </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B97" s="4">
+    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B97" s="5">
         <v>89</v>
       </c>
       <c r="C97" s="2">
@@ -2112,14 +2083,14 @@
         <v>68</v>
       </c>
       <c r="F97" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="G97" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B98" s="4">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B98" s="5">
         <v>90</v>
       </c>
       <c r="C98" s="2">
@@ -2129,14 +2100,14 @@
         <v>68</v>
       </c>
       <c r="F98" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="G98" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B99" s="4">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B99" s="5">
         <v>91</v>
       </c>
       <c r="C99" s="2">
@@ -2146,14 +2117,14 @@
         <v>68</v>
       </c>
       <c r="F99" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="G99" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B100" s="4">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B100" s="5">
         <v>92</v>
       </c>
       <c r="C100" s="2">
@@ -2163,17 +2134,17 @@
         <v>68</v>
       </c>
       <c r="F100" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G100" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="H100" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B101" s="4">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B101" s="5">
         <v>93</v>
       </c>
       <c r="C101" s="2">
@@ -2183,14 +2154,14 @@
         <v>68</v>
       </c>
       <c r="F101" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="G101" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="102" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B102" s="4">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B102" s="5">
         <v>94</v>
       </c>
       <c r="C102" s="2">
@@ -2200,14 +2171,14 @@
         <v>68</v>
       </c>
       <c r="F102" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="G102" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="103" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B103" s="4">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B103" s="5">
         <v>95</v>
       </c>
       <c r="C103" s="2">
@@ -2217,14 +2188,14 @@
         <v>68</v>
       </c>
       <c r="F103" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="G103" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="104" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B104" s="4">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B104" s="5">
         <v>96</v>
       </c>
       <c r="C104" s="2">
@@ -2234,17 +2205,17 @@
         <v>68</v>
       </c>
       <c r="F104" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G104" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="H104" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="105" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B105" s="4">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B105" s="5">
         <v>97</v>
       </c>
       <c r="C105" s="2">
@@ -2254,14 +2225,14 @@
         <v>68</v>
       </c>
       <c r="F105" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="G105" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="106" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B106" s="4">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B106" s="5">
         <v>98</v>
       </c>
       <c r="C106" s="2">
@@ -2271,14 +2242,14 @@
         <v>68</v>
       </c>
       <c r="F106" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="G106" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="107" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B107" s="4">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B107" s="5">
         <v>99</v>
       </c>
       <c r="C107" s="2">
@@ -2288,14 +2259,14 @@
         <v>68</v>
       </c>
       <c r="F107" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="G107" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="108" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B108" s="4">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B108" s="5">
         <v>100</v>
       </c>
       <c r="C108" s="2">
@@ -2305,17 +2276,17 @@
         <v>68</v>
       </c>
       <c r="F108" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="G108" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="H108" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="109" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B109" s="4">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B109" s="5">
         <v>101</v>
       </c>
       <c r="C109" s="2">
@@ -2325,14 +2296,14 @@
         <v>68</v>
       </c>
       <c r="F109" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="G109" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="110" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B110" s="4">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B110" s="5">
         <v>102</v>
       </c>
       <c r="C110" s="2">
@@ -2342,14 +2313,14 @@
         <v>68</v>
       </c>
       <c r="F110" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="G110" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="111" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B111" s="4">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B111" s="5">
         <v>103</v>
       </c>
       <c r="C111" s="2">
@@ -2359,14 +2330,14 @@
         <v>68</v>
       </c>
       <c r="F111" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="G111" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="112" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B112" s="4">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B112" s="5">
         <v>104</v>
       </c>
       <c r="C112">
@@ -2382,7 +2353,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B113" s="4">
         <v>105</v>
       </c>
@@ -2399,7 +2370,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B114" s="4">
         <v>106</v>
       </c>
@@ -2416,7 +2387,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="115" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B115" s="4">
         <v>107</v>
       </c>
@@ -2433,7 +2404,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B116" s="4">
         <v>108</v>
       </c>
@@ -2450,7 +2421,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="117" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B117" s="4">
         <v>109</v>
       </c>
@@ -2467,7 +2438,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="118" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B118" s="4">
         <v>110</v>
       </c>
@@ -2484,7 +2455,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B119" s="4">
         <v>111</v>
       </c>
@@ -2501,8 +2472,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="120" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B120" s="4">
+    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B120" s="5">
         <v>112</v>
       </c>
       <c r="C120">
@@ -2518,8 +2489,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="121" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B121" s="4">
+    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B121" s="5">
         <v>113</v>
       </c>
       <c r="C121">
@@ -2535,8 +2506,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="122" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B122" s="4">
+    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B122" s="5">
         <v>114</v>
       </c>
       <c r="C122">
@@ -2552,8 +2523,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="123" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B123" s="4">
+    <row r="123" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B123" s="5">
         <v>115</v>
       </c>
       <c r="C123">
@@ -2569,8 +2540,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="124" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B124" s="4">
+    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B124" s="5">
         <v>116</v>
       </c>
       <c r="C124">
@@ -2586,8 +2557,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="125" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B125" s="4">
+    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B125" s="5">
         <v>117</v>
       </c>
       <c r="C125">
@@ -2603,8 +2574,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="126" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B126" s="4">
+    <row r="126" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B126" s="5">
         <v>118</v>
       </c>
       <c r="C126">
@@ -2620,8 +2591,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="127" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B127" s="4">
+    <row r="127" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B127" s="5">
         <v>119</v>
       </c>
       <c r="C127">
@@ -2637,8 +2608,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="128" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B128" s="4">
+    <row r="128" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B128" s="5">
         <v>120</v>
       </c>
       <c r="C128">
@@ -2654,8 +2625,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="129" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B129" s="4">
+    <row r="129" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B129" s="5">
         <v>121</v>
       </c>
       <c r="C129">
@@ -2671,8 +2642,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="130" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B130" s="4">
+    <row r="130" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B130" s="5">
         <v>122</v>
       </c>
       <c r="C130">
@@ -2688,8 +2659,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="131" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B131" s="4">
+    <row r="131" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B131" s="5">
         <v>123</v>
       </c>
       <c r="C131">
@@ -2705,8 +2676,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="132" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B132" s="4">
+    <row r="132" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B132" s="5">
         <v>124</v>
       </c>
       <c r="C132">
@@ -2722,8 +2693,8 @@
         <v>56</v>
       </c>
     </row>
-    <row r="133" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B133" s="4">
+    <row r="133" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B133" s="5">
         <v>125</v>
       </c>
       <c r="C133">
@@ -2739,8 +2710,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="134" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B134" s="4">
+    <row r="134" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B134" s="5">
         <v>126</v>
       </c>
       <c r="C134">
@@ -2756,8 +2727,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="135" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B135" s="4">
+    <row r="135" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B135" s="5">
         <v>127</v>
       </c>
       <c r="C135">
@@ -2773,8 +2744,8 @@
         <v>59</v>
       </c>
     </row>
-    <row r="136" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B136" s="4">
+    <row r="136" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B136" s="5">
         <v>128</v>
       </c>
       <c r="C136">
@@ -2790,8 +2761,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="137" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B137" s="4">
+    <row r="137" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B137" s="5">
         <v>129</v>
       </c>
       <c r="C137">
@@ -2807,8 +2778,8 @@
         <v>61</v>
       </c>
     </row>
-    <row r="138" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B138" s="4">
+    <row r="138" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B138" s="5">
         <v>130</v>
       </c>
       <c r="C138">
@@ -2824,8 +2795,8 @@
         <v>62</v>
       </c>
     </row>
-    <row r="139" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B139" s="4">
+    <row r="139" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B139" s="5">
         <v>131</v>
       </c>
       <c r="C139">
@@ -2841,8 +2812,8 @@
         <v>63</v>
       </c>
     </row>
-    <row r="140" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B140" s="4">
+    <row r="140" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B140" s="5">
         <v>132</v>
       </c>
       <c r="C140">
@@ -2858,8 +2829,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="141" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B141" s="4">
+    <row r="141" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B141" s="5">
         <v>133</v>
       </c>
       <c r="C141">
@@ -2875,8 +2846,8 @@
         <v>65</v>
       </c>
     </row>
-    <row r="142" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B142" s="4">
+    <row r="142" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B142" s="5">
         <v>134</v>
       </c>
       <c r="C142">
@@ -2892,8 +2863,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="143" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B143" s="4">
+    <row r="143" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B143" s="5">
         <v>135</v>
       </c>
       <c r="C143">
@@ -2910,10 +2881,6 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C112:H143">
-    <sortCondition descending="1" ref="C112:C143"/>
-  </sortState>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
fix wrong bitstream order
</commit_message>
<xml_diff>
--- a/doc/bitstream_doc.xlsx
+++ b/doc/bitstream_doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Downloads\FPGA\my-discrete-fpga\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67425CD-B63C-48A2-8E91-6D852A05243D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB108E0-FC56-4951-BAAC-A1E8940C4996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14865" yWindow="0" windowWidth="13935" windowHeight="16200" xr2:uid="{C7546AD3-8A64-4A61-AF3E-FA211CF4A71C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{C7546AD3-8A64-4A61-AF3E-FA211CF4A71C}"/>
   </bookViews>
   <sheets>
     <sheet name="bitstream" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="186">
   <si>
     <t>Bitstream Documentation for one full slice</t>
   </si>
@@ -572,14 +572,35 @@
     <t>xp_ns[4]_ew[4]</t>
   </si>
   <si>
-    <t>?</t>
+    <t>en_bus_east[5]</t>
+  </si>
+  <si>
+    <t>en_bus_east[4]</t>
+  </si>
+  <si>
+    <t>en_bus_west[5]</t>
+  </si>
+  <si>
+    <t>en_bus_west[4]</t>
+  </si>
+  <si>
+    <t>en_bus_north[5]</t>
+  </si>
+  <si>
+    <t>en_bus_north[4]</t>
+  </si>
+  <si>
+    <t>en_bus_south[5]</t>
+  </si>
+  <si>
+    <t>en_bus_south[4]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -603,6 +624,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Consolas"/>
@@ -641,7 +669,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -656,6 +684,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -973,7 +1002,7 @@
   <dimension ref="A1:H139"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="G140" sqref="G140"/>
+      <selection activeCell="G109" sqref="G109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2913,7 +2942,7 @@
       <c r="E108" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F108" s="6" t="s">
+      <c r="F108" s="8" t="s">
         <v>36</v>
       </c>
       <c r="G108" s="2" t="s">
@@ -2934,7 +2963,7 @@
       <c r="E109" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F109" s="6" t="s">
+      <c r="F109" s="8" t="s">
         <v>37</v>
       </c>
       <c r="G109" s="2" t="s">
@@ -2955,7 +2984,7 @@
       <c r="E110" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F110" s="6" t="s">
+      <c r="F110" s="8" t="s">
         <v>38</v>
       </c>
       <c r="G110" s="2" t="s">
@@ -2976,7 +3005,7 @@
       <c r="E111" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F111" s="6" t="s">
+      <c r="F111" s="8" t="s">
         <v>39</v>
       </c>
       <c r="G111" s="2" t="s">
@@ -2997,7 +3026,7 @@
       <c r="E112" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F112" s="6" t="s">
+      <c r="F112" s="8" t="s">
         <v>40</v>
       </c>
       <c r="G112" s="6" t="s">
@@ -3018,7 +3047,7 @@
       <c r="E113" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F113" s="6" t="s">
+      <c r="F113" s="8" t="s">
         <v>41</v>
       </c>
       <c r="G113" s="6" t="s">
@@ -3039,7 +3068,7 @@
       <c r="E114" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F114" s="6" t="s">
+      <c r="F114" s="8" t="s">
         <v>42</v>
       </c>
       <c r="G114" s="6" t="s">
@@ -3060,7 +3089,7 @@
       <c r="E115" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F115" s="6" t="s">
+      <c r="F115" s="8" t="s">
         <v>43</v>
       </c>
       <c r="G115" s="6" t="s">
@@ -3081,10 +3110,12 @@
       <c r="E116" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F116" s="6" t="s">
+      <c r="F116" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="G116" s="2"/>
+      <c r="G116" s="6" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="4">
@@ -3100,10 +3131,12 @@
       <c r="E117" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F117" s="6" t="s">
+      <c r="F117" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="G117" s="2"/>
+      <c r="G117" s="6" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="4">
@@ -3119,10 +3152,12 @@
       <c r="E118" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F118" s="6" t="s">
+      <c r="F118" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G118" s="2"/>
+      <c r="G118" s="6" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="4">
@@ -3138,10 +3173,12 @@
       <c r="E119" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F119" s="6" t="s">
+      <c r="F119" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="G119" s="2"/>
+      <c r="G119" s="6" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="4">
@@ -3157,10 +3194,12 @@
       <c r="E120" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F120" s="6" t="s">
+      <c r="F120" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G120" s="2"/>
+      <c r="G120" s="6" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="4">
@@ -3176,10 +3215,12 @@
       <c r="E121" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F121" s="6" t="s">
+      <c r="F121" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="G121" s="2"/>
+      <c r="G121" s="6" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="4">
@@ -3195,10 +3236,12 @@
       <c r="E122" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F122" s="6" t="s">
+      <c r="F122" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="G122" s="2"/>
+      <c r="G122" s="6" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="4">
@@ -3214,10 +3257,12 @@
       <c r="E123" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F123" s="6" t="s">
+      <c r="F123" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="G123" s="2"/>
+      <c r="G123" s="6" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="4">
@@ -3233,10 +3278,12 @@
       <c r="E124" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F124" s="6" t="s">
+      <c r="F124" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="G124" s="2"/>
+      <c r="G124" s="6" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="4">
@@ -3252,10 +3299,12 @@
       <c r="E125" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F125" s="6" t="s">
+      <c r="F125" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G125" s="2"/>
+      <c r="G125" s="6" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="4">
@@ -3271,10 +3320,12 @@
       <c r="E126" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F126" s="6" t="s">
+      <c r="F126" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="G126" s="2"/>
+      <c r="G126" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="4">
@@ -3290,10 +3341,12 @@
       <c r="E127" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F127" s="6" t="s">
+      <c r="F127" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G127" s="2"/>
+      <c r="G127" s="6" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="4">
@@ -3309,10 +3362,12 @@
       <c r="E128" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F128" s="6" t="s">
+      <c r="F128" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="G128" s="2"/>
+      <c r="G128" s="6" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="4">
@@ -3328,10 +3383,12 @@
       <c r="E129" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F129" s="6" t="s">
+      <c r="F129" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="G129" s="2"/>
+      <c r="G129" s="6" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="4">
@@ -3347,10 +3404,12 @@
       <c r="E130" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F130" s="6" t="s">
+      <c r="F130" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="G130" s="2"/>
+      <c r="G130" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="4">
@@ -3366,10 +3425,12 @@
       <c r="E131" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F131" s="6" t="s">
+      <c r="F131" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="G131" s="2"/>
+      <c r="G131" s="6" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="4">
@@ -3385,10 +3446,10 @@
       <c r="E132" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F132" s="6" t="s">
+      <c r="F132" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="G132" s="2" t="s">
+      <c r="G132" s="6" t="s">
         <v>178</v>
       </c>
     </row>
@@ -3406,11 +3467,11 @@
       <c r="E133" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F133" s="6" t="s">
+      <c r="F133" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="G133" s="2" t="s">
-        <v>178</v>
+      <c r="G133" s="6" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
@@ -3427,11 +3488,11 @@
       <c r="E134" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F134" s="6" t="s">
+      <c r="F134" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="G134" s="2" t="s">
-        <v>178</v>
+      <c r="G134" s="6" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
@@ -3448,11 +3509,11 @@
       <c r="E135" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F135" s="6" t="s">
+      <c r="F135" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="G135" s="2" t="s">
-        <v>178</v>
+      <c r="G135" s="6" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
@@ -3469,11 +3530,11 @@
       <c r="E136" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F136" s="6" t="s">
+      <c r="F136" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="G136" s="2" t="s">
-        <v>178</v>
+      <c r="G136" s="6" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
@@ -3490,11 +3551,11 @@
       <c r="E137" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F137" s="6" t="s">
+      <c r="F137" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="G137" s="2" t="s">
-        <v>178</v>
+      <c r="G137" s="6" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
@@ -3511,11 +3572,11 @@
       <c r="E138" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F138" s="6" t="s">
+      <c r="F138" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="G138" s="2" t="s">
-        <v>178</v>
+      <c r="G138" s="6" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
@@ -3532,11 +3593,11 @@
       <c r="E139" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F139" s="6" t="s">
+      <c r="F139" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="G139" s="2" t="s">
-        <v>178</v>
+      <c r="G139" s="6" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated VHDL model to match PCB
</commit_message>
<xml_diff>
--- a/doc/bitstream_doc.xlsx
+++ b/doc/bitstream_doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Downloads\FPGA\my-discrete-fpga\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB108E0-FC56-4951-BAAC-A1E8940C4996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2B46D2-01D1-4395-A840-338629350A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{C7546AD3-8A64-4A61-AF3E-FA211CF4A71C}"/>
+    <workbookView xWindow="820" yWindow="-110" windowWidth="24890" windowHeight="14620" xr2:uid="{C7546AD3-8A64-4A61-AF3E-FA211CF4A71C}"/>
   </bookViews>
   <sheets>
     <sheet name="bitstream" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="188">
   <si>
     <t>Bitstream Documentation for one full slice</t>
   </si>
@@ -594,13 +594,19 @@
   </si>
   <si>
     <t>en_bus_south[4]</t>
+  </si>
+  <si>
+    <t>set_ce</t>
+  </si>
+  <si>
+    <t>slice clock enable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -629,26 +635,13 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -669,7 +662,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -678,13 +671,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1001,49 +995,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC18F46-B9E9-4D36-8A8B-C506C3DCD618}">
   <dimension ref="A1:H139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="G109" sqref="G109"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="15.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" customWidth="1"/>
-    <col min="7" max="7" width="25.85546875" customWidth="1"/>
-    <col min="8" max="8" width="59.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" style="1"/>
+    <col min="5" max="5" width="15.1796875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.1796875" customWidth="1"/>
+    <col min="7" max="7" width="25.81640625" customWidth="1"/>
+    <col min="8" max="8" width="59.54296875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:7" s="4" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="3">
         <v>0</v>
       </c>
       <c r="B4">
@@ -1053,16 +1047,16 @@
       <c r="D4" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>84</v>
       </c>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="3">
         <v>1</v>
       </c>
       <c r="B5">
@@ -1072,16 +1066,16 @@
       <c r="D5" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>82</v>
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="3">
         <v>2</v>
       </c>
       <c r="B6">
@@ -1091,16 +1085,16 @@
       <c r="D6" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>83</v>
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="3">
         <v>3</v>
       </c>
       <c r="B7">
@@ -1110,16 +1104,16 @@
       <c r="D7" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>81</v>
       </c>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="3">
         <v>4</v>
       </c>
       <c r="B8">
@@ -1129,16 +1123,16 @@
       <c r="D8" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>64</v>
       </c>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="3">
         <v>5</v>
       </c>
       <c r="B9">
@@ -1148,16 +1142,16 @@
       <c r="D9" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="5" t="s">
         <v>65</v>
       </c>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="3">
         <v>6</v>
       </c>
       <c r="B10">
@@ -1167,16 +1161,16 @@
       <c r="D10" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>66</v>
       </c>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="3">
         <v>7</v>
       </c>
       <c r="B11">
@@ -1186,16 +1180,16 @@
       <c r="D11" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>67</v>
       </c>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="3">
         <v>8</v>
       </c>
       <c r="B12">
@@ -1205,18 +1199,18 @@
       <c r="D12" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="E12" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="3">
         <v>9</v>
       </c>
       <c r="B13">
@@ -1226,18 +1220,18 @@
       <c r="D13" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="3">
         <v>10</v>
       </c>
       <c r="B14">
@@ -1247,18 +1241,18 @@
       <c r="D14" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="5" t="s">
         <v>111</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="3">
         <v>11</v>
       </c>
       <c r="B15">
@@ -1268,18 +1262,18 @@
       <c r="D15" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="5" t="s">
         <v>109</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="3">
         <v>12</v>
       </c>
       <c r="B16">
@@ -1289,18 +1283,18 @@
       <c r="D16" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="5" t="s">
         <v>107</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="3">
         <v>13</v>
       </c>
       <c r="B17">
@@ -1310,18 +1304,18 @@
       <c r="D17" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="5" t="s">
         <v>106</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="3">
         <v>14</v>
       </c>
       <c r="B18">
@@ -1331,18 +1325,18 @@
       <c r="D18" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="5" t="s">
         <v>105</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="3">
         <v>15</v>
       </c>
       <c r="B19">
@@ -1352,18 +1346,18 @@
       <c r="D19" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="5" t="s">
         <v>104</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="3">
         <v>16</v>
       </c>
       <c r="B20">
@@ -1373,14 +1367,14 @@
       <c r="D20" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
       <c r="G20" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="3">
         <v>17</v>
       </c>
       <c r="B21">
@@ -1390,14 +1384,14 @@
       <c r="D21" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
       <c r="G21" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="3">
         <v>18</v>
       </c>
       <c r="B22">
@@ -1407,14 +1401,14 @@
       <c r="D22" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
       <c r="G22" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="3">
         <v>19</v>
       </c>
       <c r="B23">
@@ -1424,14 +1418,14 @@
       <c r="D23" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
       <c r="G23" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="3">
         <v>20</v>
       </c>
       <c r="B24">
@@ -1441,14 +1435,14 @@
       <c r="D24" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
       <c r="G24" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="3">
         <v>21</v>
       </c>
       <c r="B25">
@@ -1458,14 +1452,14 @@
       <c r="D25" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
       <c r="G25" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="3">
         <v>22</v>
       </c>
       <c r="B26">
@@ -1475,14 +1469,14 @@
       <c r="D26" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
       <c r="G26" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="3">
         <v>23</v>
       </c>
       <c r="B27">
@@ -1492,16 +1486,16 @@
       <c r="D27" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6" t="s">
+      <c r="E27" s="5"/>
+      <c r="F27" s="5" t="s">
         <v>150</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="3">
         <v>24</v>
       </c>
       <c r="B28">
@@ -1511,14 +1505,14 @@
       <c r="D28" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
       <c r="G28" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" s="3">
         <v>25</v>
       </c>
       <c r="B29">
@@ -1528,14 +1522,14 @@
       <c r="D29" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
       <c r="G29" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" s="3">
         <v>26</v>
       </c>
       <c r="B30">
@@ -1545,14 +1539,14 @@
       <c r="D30" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
       <c r="G30" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" s="3">
         <v>27</v>
       </c>
       <c r="B31">
@@ -1562,14 +1556,14 @@
       <c r="D31" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
       <c r="G31" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" s="3">
         <v>28</v>
       </c>
       <c r="B32">
@@ -1579,14 +1573,14 @@
       <c r="D32" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
       <c r="G32" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" s="3">
         <v>29</v>
       </c>
       <c r="B33">
@@ -1596,14 +1590,14 @@
       <c r="D33" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
       <c r="G33" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="3">
         <v>30</v>
       </c>
       <c r="B34">
@@ -1613,14 +1607,14 @@
       <c r="D34" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
       <c r="G34" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" s="3">
         <v>31</v>
       </c>
       <c r="B35">
@@ -1630,16 +1624,16 @@
       <c r="D35" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6" t="s">
+      <c r="E35" s="5"/>
+      <c r="F35" s="5" t="s">
         <v>149</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" s="3">
         <v>32</v>
       </c>
       <c r="B36">
@@ -1649,14 +1643,14 @@
       <c r="D36" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
       <c r="G36" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="3">
         <v>33</v>
       </c>
       <c r="B37">
@@ -1666,14 +1660,14 @@
       <c r="D37" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
       <c r="G37" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" s="3">
         <v>34</v>
       </c>
       <c r="B38">
@@ -1683,14 +1677,14 @@
       <c r="D38" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
       <c r="G38" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" s="3">
         <v>35</v>
       </c>
       <c r="B39">
@@ -1700,14 +1694,14 @@
       <c r="D39" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
       <c r="G39" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="4">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" s="3">
         <v>36</v>
       </c>
       <c r="B40">
@@ -1717,14 +1711,14 @@
       <c r="D40" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
       <c r="G40" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="4">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" s="3">
         <v>37</v>
       </c>
       <c r="B41">
@@ -1734,14 +1728,14 @@
       <c r="D41" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
       <c r="G41" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="4">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" s="3">
         <v>38</v>
       </c>
       <c r="B42">
@@ -1751,14 +1745,14 @@
       <c r="D42" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
       <c r="G42" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="4">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" s="3">
         <v>39</v>
       </c>
       <c r="B43">
@@ -1768,16 +1762,16 @@
       <c r="D43" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6" t="s">
+      <c r="E43" s="5"/>
+      <c r="F43" s="5" t="s">
         <v>148</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="4">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" s="3">
         <v>40</v>
       </c>
       <c r="B44">
@@ -1787,14 +1781,14 @@
       <c r="D44" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
       <c r="G44" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="4">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" s="3">
         <v>41</v>
       </c>
       <c r="B45">
@@ -1804,14 +1798,14 @@
       <c r="D45" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
       <c r="G45" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" s="3">
         <v>42</v>
       </c>
       <c r="B46">
@@ -1821,14 +1815,14 @@
       <c r="D46" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
       <c r="G46" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" s="3">
         <v>43</v>
       </c>
       <c r="B47">
@@ -1838,14 +1832,14 @@
       <c r="D47" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
       <c r="G47" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="4">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48" s="3">
         <v>44</v>
       </c>
       <c r="B48">
@@ -1855,14 +1849,14 @@
       <c r="D48" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
       <c r="G48" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="4">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A49" s="3">
         <v>45</v>
       </c>
       <c r="B49">
@@ -1872,14 +1866,14 @@
       <c r="D49" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
       <c r="G49" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="4">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A50" s="3">
         <v>46</v>
       </c>
       <c r="B50">
@@ -1889,14 +1883,14 @@
       <c r="D50" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
       <c r="G50" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="4">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51" s="3">
         <v>47</v>
       </c>
       <c r="B51">
@@ -1906,16 +1900,16 @@
       <c r="D51" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6" t="s">
+      <c r="E51" s="5"/>
+      <c r="F51" s="5" t="s">
         <v>147</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="4">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A52" s="3">
         <v>48</v>
       </c>
       <c r="B52">
@@ -1925,14 +1919,14 @@
       <c r="D52" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
       <c r="G52" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="4">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A53" s="3">
         <v>49</v>
       </c>
       <c r="B53">
@@ -1942,14 +1936,14 @@
       <c r="D53" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E53" s="6"/>
-      <c r="F53" s="6"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
       <c r="G53" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="4">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A54" s="3">
         <v>50</v>
       </c>
       <c r="B54">
@@ -1959,14 +1953,14 @@
       <c r="D54" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E54" s="6"/>
-      <c r="F54" s="6"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
       <c r="G54" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="4">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A55" s="3">
         <v>51</v>
       </c>
       <c r="B55">
@@ -1976,14 +1970,14 @@
       <c r="D55" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E55" s="6"/>
-      <c r="F55" s="6"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
       <c r="G55" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="4">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A56" s="3">
         <v>52</v>
       </c>
       <c r="B56">
@@ -1993,14 +1987,14 @@
       <c r="D56" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E56" s="6"/>
-      <c r="F56" s="6"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
       <c r="G56" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="4">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A57" s="3">
         <v>53</v>
       </c>
       <c r="B57">
@@ -2010,14 +2004,14 @@
       <c r="D57" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E57" s="6"/>
-      <c r="F57" s="6"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
       <c r="G57" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="4">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A58" s="3">
         <v>54</v>
       </c>
       <c r="B58">
@@ -2027,14 +2021,14 @@
       <c r="D58" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E58" s="6"/>
-      <c r="F58" s="6"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
       <c r="G58" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="4">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59" s="3">
         <v>55</v>
       </c>
       <c r="B59">
@@ -2044,16 +2038,16 @@
       <c r="D59" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E59" s="6"/>
-      <c r="F59" s="6" t="s">
+      <c r="E59" s="5"/>
+      <c r="F59" s="5" t="s">
         <v>146</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="4">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A60" s="3">
         <v>56</v>
       </c>
       <c r="B60">
@@ -2063,14 +2057,14 @@
       <c r="D60" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E60" s="6"/>
-      <c r="F60" s="6"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
       <c r="G60" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="4">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A61" s="3">
         <v>57</v>
       </c>
       <c r="B61">
@@ -2080,14 +2074,14 @@
       <c r="D61" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E61" s="6"/>
-      <c r="F61" s="6"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
       <c r="G61" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="4">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A62" s="3">
         <v>58</v>
       </c>
       <c r="B62">
@@ -2097,14 +2091,14 @@
       <c r="D62" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E62" s="6"/>
-      <c r="F62" s="6"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
       <c r="G62" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="4">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A63" s="3">
         <v>59</v>
       </c>
       <c r="B63">
@@ -2114,14 +2108,14 @@
       <c r="D63" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E63" s="6"/>
-      <c r="F63" s="6"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
       <c r="G63" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="4">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A64" s="3">
         <v>60</v>
       </c>
       <c r="B64">
@@ -2131,14 +2125,14 @@
       <c r="D64" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E64" s="6"/>
-      <c r="F64" s="6"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
       <c r="G64" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="4">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A65" s="3">
         <v>61</v>
       </c>
       <c r="B65">
@@ -2148,14 +2142,14 @@
       <c r="D65" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E65" s="6"/>
-      <c r="F65" s="6"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
       <c r="G65" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="4">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A66" s="3">
         <v>62</v>
       </c>
       <c r="B66">
@@ -2165,14 +2159,14 @@
       <c r="D66" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E66" s="6"/>
-      <c r="F66" s="6"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
       <c r="G66" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="4">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A67" s="3">
         <v>63</v>
       </c>
       <c r="B67">
@@ -2182,16 +2176,16 @@
       <c r="D67" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E67" s="6"/>
-      <c r="F67" s="6" t="s">
+      <c r="E67" s="5"/>
+      <c r="F67" s="5" t="s">
         <v>145</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="4">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A68" s="3">
         <v>64</v>
       </c>
       <c r="B68">
@@ -2201,14 +2195,14 @@
       <c r="D68" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E68" s="6"/>
-      <c r="F68" s="6"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
       <c r="G68" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="4">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A69" s="3">
         <v>65</v>
       </c>
       <c r="B69">
@@ -2218,14 +2212,14 @@
       <c r="D69" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E69" s="6"/>
-      <c r="F69" s="6"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
       <c r="G69" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="4">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A70" s="3">
         <v>66</v>
       </c>
       <c r="B70">
@@ -2235,14 +2229,14 @@
       <c r="D70" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E70" s="6"/>
-      <c r="F70" s="6"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
       <c r="G70" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="4">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A71" s="3">
         <v>67</v>
       </c>
       <c r="B71">
@@ -2252,14 +2246,14 @@
       <c r="D71" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E71" s="6"/>
-      <c r="F71" s="6"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
       <c r="G71" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="4">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A72" s="3">
         <v>68</v>
       </c>
       <c r="B72">
@@ -2269,14 +2263,14 @@
       <c r="D72" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E72" s="6"/>
-      <c r="F72" s="6"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
       <c r="G72" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="4">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A73" s="3">
         <v>69</v>
       </c>
       <c r="B73">
@@ -2286,14 +2280,14 @@
       <c r="D73" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E73" s="6"/>
-      <c r="F73" s="6"/>
+      <c r="E73" s="5"/>
+      <c r="F73" s="5"/>
       <c r="G73" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="4">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A74" s="3">
         <v>70</v>
       </c>
       <c r="B74">
@@ -2303,14 +2297,14 @@
       <c r="D74" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E74" s="6"/>
-      <c r="F74" s="6"/>
+      <c r="E74" s="5"/>
+      <c r="F74" s="5"/>
       <c r="G74" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="4">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A75" s="3">
         <v>71</v>
       </c>
       <c r="B75">
@@ -2320,16 +2314,16 @@
       <c r="D75" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E75" s="6"/>
-      <c r="F75" s="6" t="s">
+      <c r="E75" s="5"/>
+      <c r="F75" s="5" t="s">
         <v>144</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="4">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A76" s="3">
         <v>72</v>
       </c>
       <c r="B76">
@@ -2339,14 +2333,14 @@
       <c r="D76" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E76" s="6"/>
-      <c r="F76" s="6"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
       <c r="G76" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="4">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A77" s="3">
         <v>73</v>
       </c>
       <c r="B77">
@@ -2356,14 +2350,14 @@
       <c r="D77" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E77" s="6"/>
-      <c r="F77" s="6"/>
+      <c r="E77" s="5"/>
+      <c r="F77" s="5"/>
       <c r="G77" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="4">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A78" s="3">
         <v>74</v>
       </c>
       <c r="B78">
@@ -2373,14 +2367,14 @@
       <c r="D78" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E78" s="6"/>
-      <c r="F78" s="6"/>
+      <c r="E78" s="5"/>
+      <c r="F78" s="5"/>
       <c r="G78" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="4">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A79" s="3">
         <v>75</v>
       </c>
       <c r="B79">
@@ -2390,14 +2384,14 @@
       <c r="D79" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E79" s="6"/>
-      <c r="F79" s="6"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="5"/>
       <c r="G79" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="4">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A80" s="3">
         <v>76</v>
       </c>
       <c r="B80">
@@ -2407,14 +2401,14 @@
       <c r="D80" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E80" s="6"/>
-      <c r="F80" s="6"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="5"/>
       <c r="G80" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="4">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A81" s="3">
         <v>77</v>
       </c>
       <c r="B81">
@@ -2424,14 +2418,14 @@
       <c r="D81" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E81" s="6"/>
-      <c r="F81" s="6"/>
+      <c r="E81" s="5"/>
+      <c r="F81" s="5"/>
       <c r="G81" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="4">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A82" s="3">
         <v>78</v>
       </c>
       <c r="B82">
@@ -2441,14 +2435,14 @@
       <c r="D82" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E82" s="6"/>
-      <c r="F82" s="6"/>
+      <c r="E82" s="5"/>
+      <c r="F82" s="5"/>
       <c r="G82" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="4">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A83" s="3">
         <v>79</v>
       </c>
       <c r="B83">
@@ -2458,16 +2452,16 @@
       <c r="D83" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E83" s="6"/>
-      <c r="F83" s="6" t="s">
+      <c r="E83" s="5"/>
+      <c r="F83" s="5" t="s">
         <v>143</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="4">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A84" s="3">
         <v>80</v>
       </c>
       <c r="B84">
@@ -2477,16 +2471,16 @@
       <c r="D84" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E84" s="6" t="s">
+      <c r="E84" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="F84" s="6" t="s">
+      <c r="F84" s="5" t="s">
         <v>103</v>
       </c>
       <c r="G84" s="2"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="4">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A85" s="3">
         <v>81</v>
       </c>
       <c r="B85">
@@ -2496,16 +2490,16 @@
       <c r="D85" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E85" s="6" t="s">
+      <c r="E85" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="F85" s="6" t="s">
+      <c r="F85" s="5" t="s">
         <v>103</v>
       </c>
       <c r="G85" s="2"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="4">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A86" s="3">
         <v>82</v>
       </c>
       <c r="B86">
@@ -2515,16 +2509,16 @@
       <c r="D86" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E86" s="6" t="s">
+      <c r="E86" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="F86" s="6" t="s">
+      <c r="F86" s="5" t="s">
         <v>102</v>
       </c>
       <c r="G86" s="2"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="4">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A87" s="3">
         <v>83</v>
       </c>
       <c r="B87">
@@ -2534,16 +2528,16 @@
       <c r="D87" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E87" s="6" t="s">
+      <c r="E87" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F87" s="6" t="s">
+      <c r="F87" s="5" t="s">
         <v>102</v>
       </c>
       <c r="G87" s="2"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="4">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A88" s="3">
         <v>84</v>
       </c>
       <c r="B88">
@@ -2553,16 +2547,16 @@
       <c r="D88" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E88" s="6" t="s">
+      <c r="E88" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="F88" s="6" t="s">
+      <c r="F88" s="5" t="s">
         <v>101</v>
       </c>
       <c r="G88" s="2"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="4">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A89" s="3">
         <v>85</v>
       </c>
       <c r="B89">
@@ -2572,16 +2566,16 @@
       <c r="D89" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E89" s="6" t="s">
+      <c r="E89" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F89" s="6" t="s">
+      <c r="F89" s="5" t="s">
         <v>101</v>
       </c>
       <c r="G89" s="2"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="4">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A90" s="3">
         <v>86</v>
       </c>
       <c r="B90">
@@ -2591,16 +2585,16 @@
       <c r="D90" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E90" s="6" t="s">
+      <c r="E90" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="F90" s="6" t="s">
+      <c r="F90" s="5" t="s">
         <v>100</v>
       </c>
       <c r="G90" s="2"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="4">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A91" s="3">
         <v>87</v>
       </c>
       <c r="B91">
@@ -2610,16 +2604,16 @@
       <c r="D91" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E91" s="6" t="s">
+      <c r="E91" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F91" s="6" t="s">
+      <c r="F91" s="5" t="s">
         <v>100</v>
       </c>
       <c r="G91" s="2"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="4">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A92" s="3">
         <v>88</v>
       </c>
       <c r="B92" s="1">
@@ -2629,16 +2623,16 @@
       <c r="D92" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E92" s="7" t="s">
+      <c r="E92" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F92" s="6" t="s">
+      <c r="F92" s="5" t="s">
         <v>112</v>
       </c>
       <c r="G92" s="2"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="4">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A93" s="3">
         <v>89</v>
       </c>
       <c r="B93" s="1">
@@ -2648,16 +2642,16 @@
       <c r="D93" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E93" s="6" t="s">
+      <c r="E93" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="F93" s="6" t="s">
+      <c r="F93" s="5" t="s">
         <v>152</v>
       </c>
       <c r="G93" s="2"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="4">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A94" s="3">
         <v>90</v>
       </c>
       <c r="B94" s="1">
@@ -2667,16 +2661,16 @@
       <c r="D94" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E94" s="6" t="s">
+      <c r="E94" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="F94" s="6" t="s">
+      <c r="F94" s="5" t="s">
         <v>151</v>
       </c>
       <c r="G94" s="2"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="4">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A95" s="3">
         <v>91</v>
       </c>
       <c r="B95" s="1">
@@ -2686,16 +2680,16 @@
       <c r="D95" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E95" s="6" t="s">
+      <c r="E95" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="F95" s="6" t="s">
+      <c r="F95" s="5" t="s">
         <v>153</v>
       </c>
       <c r="G95" s="2"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="4">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A96" s="3">
         <v>92</v>
       </c>
       <c r="B96" s="1">
@@ -2705,18 +2699,18 @@
       <c r="D96" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E96" s="6" t="s">
+      <c r="E96" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="F96" s="6" t="s">
+      <c r="F96" s="5" t="s">
         <v>128</v>
       </c>
       <c r="G96" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="4">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A97" s="3">
         <v>93</v>
       </c>
       <c r="B97" s="1">
@@ -2726,16 +2720,16 @@
       <c r="D97" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E97" s="6" t="s">
+      <c r="E97" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="F97" s="6" t="s">
+      <c r="F97" s="5" t="s">
         <v>142</v>
       </c>
       <c r="G97" s="2"/>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="4">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A98" s="3">
         <v>94</v>
       </c>
       <c r="B98" s="1">
@@ -2745,16 +2739,16 @@
       <c r="D98" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E98" s="6" t="s">
+      <c r="E98" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F98" s="6" t="s">
+      <c r="F98" s="5" t="s">
         <v>141</v>
       </c>
       <c r="G98" s="2"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="4">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A99" s="3">
         <v>95</v>
       </c>
       <c r="B99" s="1">
@@ -2764,16 +2758,16 @@
       <c r="D99" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E99" s="6" t="s">
+      <c r="E99" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="F99" s="6" t="s">
+      <c r="F99" s="5" t="s">
         <v>140</v>
       </c>
       <c r="G99" s="2"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="4">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A100" s="3">
         <v>96</v>
       </c>
       <c r="B100" s="1">
@@ -2783,18 +2777,18 @@
       <c r="D100" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E100" s="6" t="s">
+      <c r="E100" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="F100" s="6" t="s">
+      <c r="F100" s="5" t="s">
         <v>130</v>
       </c>
       <c r="G100" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="4">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A101" s="3">
         <v>97</v>
       </c>
       <c r="B101" s="1">
@@ -2804,16 +2798,16 @@
       <c r="D101" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E101" s="6" t="s">
+      <c r="E101" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="F101" s="6" t="s">
+      <c r="F101" s="5" t="s">
         <v>139</v>
       </c>
       <c r="G101" s="2"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="4">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A102" s="3">
         <v>98</v>
       </c>
       <c r="B102" s="1">
@@ -2823,16 +2817,16 @@
       <c r="D102" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E102" s="6" t="s">
+      <c r="E102" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F102" s="6" t="s">
+      <c r="F102" s="5" t="s">
         <v>138</v>
       </c>
       <c r="G102" s="2"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="4">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A103" s="3">
         <v>99</v>
       </c>
       <c r="B103" s="1">
@@ -2842,16 +2836,16 @@
       <c r="D103" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E103" s="6" t="s">
+      <c r="E103" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="F103" s="6" t="s">
+      <c r="F103" s="5" t="s">
         <v>137</v>
       </c>
       <c r="G103" s="2"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="4">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A104" s="3">
         <v>100</v>
       </c>
       <c r="B104" s="1">
@@ -2861,18 +2855,18 @@
       <c r="D104" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E104" s="6" t="s">
+      <c r="E104" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="F104" s="6" t="s">
+      <c r="F104" s="5" t="s">
         <v>131</v>
       </c>
       <c r="G104" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="4">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A105" s="3">
         <v>101</v>
       </c>
       <c r="B105" s="1">
@@ -2882,16 +2876,16 @@
       <c r="D105" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E105" s="6" t="s">
+      <c r="E105" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="F105" s="6" t="s">
+      <c r="F105" s="5" t="s">
         <v>136</v>
       </c>
       <c r="G105" s="2"/>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="4">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A106" s="3">
         <v>102</v>
       </c>
       <c r="B106" s="1">
@@ -2901,16 +2895,16 @@
       <c r="D106" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E106" s="6" t="s">
+      <c r="E106" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="F106" s="6" t="s">
+      <c r="F106" s="5" t="s">
         <v>135</v>
       </c>
       <c r="G106" s="2"/>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="4">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A107" s="3">
         <v>103</v>
       </c>
       <c r="B107" s="1">
@@ -2920,16 +2914,16 @@
       <c r="D107" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E107" s="6" t="s">
+      <c r="E107" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="F107" s="6" t="s">
+      <c r="F107" s="5" t="s">
         <v>134</v>
       </c>
       <c r="G107" s="2"/>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="4">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A108" s="3">
         <v>104</v>
       </c>
       <c r="B108">
@@ -2939,17 +2933,17 @@
       <c r="D108" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E108" s="6" t="s">
+      <c r="E108" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F108" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="G108" s="2" t="s">
+      <c r="F108" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G108" s="7" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A109" s="3">
         <v>105</v>
       </c>
@@ -2960,17 +2954,17 @@
       <c r="D109" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E109" s="6" t="s">
+      <c r="E109" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F109" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="G109" s="2" t="s">
+      <c r="F109" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G109" s="7" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A110" s="3">
         <v>106</v>
       </c>
@@ -2981,17 +2975,17 @@
       <c r="D110" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E110" s="6" t="s">
+      <c r="E110" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F110" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G110" s="2" t="s">
+      <c r="F110" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G110" s="7" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A111" s="3">
         <v>107</v>
       </c>
@@ -3002,17 +2996,17 @@
       <c r="D111" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E111" s="6" t="s">
+      <c r="E111" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F111" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="G111" s="2" t="s">
+      <c r="F111" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G111" s="7" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A112" s="3">
         <v>108</v>
       </c>
@@ -3023,17 +3017,17 @@
       <c r="D112" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E112" s="6" t="s">
+      <c r="E112" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F112" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="G112" s="6" t="s">
+      <c r="F112" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G112" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A113" s="3">
         <v>109</v>
       </c>
@@ -3044,17 +3038,17 @@
       <c r="D113" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E113" s="6" t="s">
+      <c r="E113" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F113" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G113" s="6" t="s">
+      <c r="F113" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G113" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A114" s="3">
         <v>110</v>
       </c>
@@ -3065,17 +3059,17 @@
       <c r="D114" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E114" s="6" t="s">
+      <c r="E114" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F114" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G114" s="6" t="s">
+      <c r="F114" s="5" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G114" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A115" s="3">
         <v>111</v>
       </c>
@@ -3086,18 +3080,18 @@
       <c r="D115" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E115" s="6" t="s">
+      <c r="E115" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F115" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G115" s="6" t="s">
+      <c r="F115" s="5" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A116" s="4">
+      <c r="G115" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A116" s="3">
         <v>112</v>
       </c>
       <c r="B116">
@@ -3107,18 +3101,18 @@
       <c r="D116" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E116" s="6" t="s">
+      <c r="E116" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F116" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G116" s="6" t="s">
+      <c r="F116" s="5" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A117" s="4">
+      <c r="G116" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A117" s="3">
         <v>113</v>
       </c>
       <c r="B117">
@@ -3128,18 +3122,18 @@
       <c r="D117" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E117" s="6" t="s">
+      <c r="E117" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F117" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G117" s="6" t="s">
+      <c r="F117" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A118" s="4">
+      <c r="G117" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A118" s="3">
         <v>114</v>
       </c>
       <c r="B118">
@@ -3149,18 +3143,18 @@
       <c r="D118" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E118" s="6" t="s">
+      <c r="E118" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F118" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G118" s="6" t="s">
+      <c r="F118" s="5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A119" s="4">
+      <c r="G118" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A119" s="3">
         <v>115</v>
       </c>
       <c r="B119">
@@ -3170,18 +3164,18 @@
       <c r="D119" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E119" s="6" t="s">
+      <c r="E119" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F119" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="G119" s="6" t="s">
+      <c r="F119" s="5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A120" s="4">
+      <c r="G119" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A120" s="3">
         <v>116</v>
       </c>
       <c r="B120">
@@ -3191,18 +3185,18 @@
       <c r="D120" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E120" s="6" t="s">
+      <c r="E120" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F120" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G120" s="6" t="s">
+      <c r="F120" s="5" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A121" s="4">
+      <c r="G120" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A121" s="3">
         <v>117</v>
       </c>
       <c r="B121">
@@ -3212,18 +3206,18 @@
       <c r="D121" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E121" s="6" t="s">
+      <c r="E121" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F121" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G121" s="6" t="s">
+      <c r="F121" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A122" s="4">
+      <c r="G121" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A122" s="3">
         <v>118</v>
       </c>
       <c r="B122">
@@ -3233,18 +3227,18 @@
       <c r="D122" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E122" s="6" t="s">
+      <c r="E122" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F122" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G122" s="6" t="s">
+      <c r="F122" s="5" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A123" s="4">
+      <c r="G122" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A123" s="3">
         <v>119</v>
       </c>
       <c r="B123">
@@ -3254,18 +3248,18 @@
       <c r="D123" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E123" s="6" t="s">
+      <c r="E123" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F123" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G123" s="6" t="s">
+      <c r="F123" s="5" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A124" s="4">
+      <c r="G123" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A124" s="3">
         <v>120</v>
       </c>
       <c r="B124">
@@ -3275,18 +3269,18 @@
       <c r="D124" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E124" s="6" t="s">
+      <c r="E124" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F124" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G124" s="6" t="s">
+      <c r="F124" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A125" s="4">
+      <c r="G124" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A125" s="3">
         <v>121</v>
       </c>
       <c r="B125">
@@ -3296,18 +3290,18 @@
       <c r="D125" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E125" s="6" t="s">
+      <c r="E125" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F125" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="G125" s="6" t="s">
+      <c r="F125" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A126" s="4">
+      <c r="G125" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A126" s="3">
         <v>122</v>
       </c>
       <c r="B126">
@@ -3317,18 +3311,18 @@
       <c r="D126" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E126" s="6" t="s">
+      <c r="E126" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F126" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="G126" s="6" t="s">
+      <c r="F126" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A127" s="4">
+      <c r="G126" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A127" s="3">
         <v>123</v>
       </c>
       <c r="B127">
@@ -3338,18 +3332,18 @@
       <c r="D127" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E127" s="6" t="s">
+      <c r="E127" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F127" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="G127" s="6" t="s">
+      <c r="F127" s="5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A128" s="4">
+      <c r="G127" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A128" s="3">
         <v>124</v>
       </c>
       <c r="B128">
@@ -3359,18 +3353,18 @@
       <c r="D128" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E128" s="6" t="s">
+      <c r="E128" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F128" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="G128" s="6" t="s">
+      <c r="F128" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A129" s="4">
+      <c r="G128" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A129" s="3">
         <v>125</v>
       </c>
       <c r="B129">
@@ -3380,18 +3374,18 @@
       <c r="D129" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E129" s="6" t="s">
+      <c r="E129" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F129" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="G129" s="6" t="s">
+      <c r="F129" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A130" s="4">
+      <c r="G129" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A130" s="3">
         <v>126</v>
       </c>
       <c r="B130">
@@ -3401,18 +3395,18 @@
       <c r="D130" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E130" s="6" t="s">
+      <c r="E130" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F130" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G130" s="6" t="s">
+      <c r="F130" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A131" s="4">
+      <c r="G130" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A131" s="3">
         <v>127</v>
       </c>
       <c r="B131">
@@ -3422,18 +3416,18 @@
       <c r="D131" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E131" s="6" t="s">
+      <c r="E131" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F131" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="G131" s="6" t="s">
+      <c r="F131" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A132" s="4">
+      <c r="G131" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A132" s="3">
         <v>128</v>
       </c>
       <c r="B132">
@@ -3443,18 +3437,18 @@
       <c r="D132" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E132" s="6" t="s">
+      <c r="E132" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F132" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G132" s="6" t="s">
+      <c r="F132" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G132" s="5" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A133" s="4">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A133" s="3">
         <v>129</v>
       </c>
       <c r="B133">
@@ -3464,18 +3458,18 @@
       <c r="D133" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E133" s="6" t="s">
+      <c r="E133" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F133" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="G133" s="6" t="s">
+      <c r="F133" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G133" s="5" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A134" s="4">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A134" s="3">
         <v>130</v>
       </c>
       <c r="B134">
@@ -3485,18 +3479,18 @@
       <c r="D134" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E134" s="6" t="s">
+      <c r="E134" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F134" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G134" s="6" t="s">
+      <c r="F134" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G134" s="5" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A135" s="4">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A135" s="3">
         <v>131</v>
       </c>
       <c r="B135">
@@ -3506,18 +3500,18 @@
       <c r="D135" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E135" s="6" t="s">
+      <c r="E135" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F135" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="G135" s="6" t="s">
+      <c r="F135" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G135" s="5" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A136" s="4">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A136" s="3">
         <v>132</v>
       </c>
       <c r="B136">
@@ -3527,18 +3521,18 @@
       <c r="D136" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E136" s="6" t="s">
+      <c r="E136" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F136" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="G136" s="6" t="s">
+      <c r="F136" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G136" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A137" s="4">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A137" s="3">
         <v>133</v>
       </c>
       <c r="B137">
@@ -3548,18 +3542,18 @@
       <c r="D137" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E137" s="6" t="s">
+      <c r="E137" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F137" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="G137" s="6" t="s">
+      <c r="F137" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G137" s="5" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A138" s="4">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A138" s="3">
         <v>134</v>
       </c>
       <c r="B138">
@@ -3569,18 +3563,18 @@
       <c r="D138" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E138" s="6" t="s">
+      <c r="E138" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F138" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="G138" s="6" t="s">
+      <c r="F138" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G138" s="5" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A139" s="4">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A139" s="3">
         <v>135</v>
       </c>
       <c r="B139">
@@ -3590,13 +3584,13 @@
       <c r="D139" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E139" s="6" t="s">
+      <c r="E139" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F139" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G139" s="6" t="s">
+      <c r="F139" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G139" s="5" t="s">
         <v>185</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed CE throughout simulation
</commit_message>
<xml_diff>
--- a/doc/bitstream_doc.xlsx
+++ b/doc/bitstream_doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Downloads\FPGA\my-discrete-fpga\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264AEC45-F029-4CDE-BBE7-CA9E9C8DA5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5AEF79-0008-4C1B-8154-77285AEC501A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="-110" windowWidth="24890" windowHeight="14620" xr2:uid="{C7546AD3-8A64-4A61-AF3E-FA211CF4A71C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{C7546AD3-8A64-4A61-AF3E-FA211CF4A71C}"/>
   </bookViews>
   <sheets>
     <sheet name="bitstream" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="191">
   <si>
     <t>Bitstream Documentation for one full slice</t>
   </si>
@@ -600,6 +600,15 @@
   </si>
   <si>
     <t>slice clock enable</t>
+  </si>
+  <si>
+    <t>xpoint_cout_ce</t>
+  </si>
+  <si>
+    <t>connect ce to bus[5]</t>
+  </si>
+  <si>
+    <t>en_ce</t>
   </si>
 </sst>
 </file>
@@ -995,8 +1004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC18F46-B9E9-4D36-8A8B-C506C3DCD618}">
   <dimension ref="A1:H139"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="F93" sqref="F93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2623,13 +2632,15 @@
       <c r="D92" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E92" s="6" t="s">
-        <v>69</v>
+      <c r="E92" s="5" t="s">
+        <v>188</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="G92" s="2"/>
+        <v>190</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93" s="3">

</xml_diff>

<commit_message>
remove final occurrences of the word "prio"
</commit_message>
<xml_diff>
--- a/doc/bitstream_doc.xlsx
+++ b/doc/bitstream_doc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Downloads\FPGA\my-discrete-fpga\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5AEF79-0008-4C1B-8154-77285AEC501A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D319443A-5EB1-4F2E-B9F5-BE8771DA5611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{C7546AD3-8A64-4A61-AF3E-FA211CF4A71C}"/>
+    <workbookView xWindow="13260" yWindow="0" windowWidth="12340" windowHeight="14400" xr2:uid="{C7546AD3-8A64-4A61-AF3E-FA211CF4A71C}"/>
   </bookViews>
   <sheets>
     <sheet name="bitstream" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="179">
   <si>
     <t>Bitstream Documentation for one full slice</t>
   </si>
@@ -146,30 +146,6 @@
     <t>SW</t>
   </si>
   <si>
-    <t>en_prio_east[1]</t>
-  </si>
-  <si>
-    <t>en_prio_east[0]</t>
-  </si>
-  <si>
-    <t>en_prio_west[1]</t>
-  </si>
-  <si>
-    <t>en_prio_west[0]</t>
-  </si>
-  <si>
-    <t>en_prio_north[1]</t>
-  </si>
-  <si>
-    <t>en_prio_north[0]</t>
-  </si>
-  <si>
-    <t>en_prio_south[1]</t>
-  </si>
-  <si>
-    <t>en_prio_south[0]</t>
-  </si>
-  <si>
     <t>en_bus_east[1]</t>
   </si>
   <si>
@@ -218,18 +194,6 @@
     <t>en_bus_south[0]</t>
   </si>
   <si>
-    <t>xp_prio_ns[1]_ew[1]</t>
-  </si>
-  <si>
-    <t>xp_prio_ns[0]_ew[1]</t>
-  </si>
-  <si>
-    <t>xp_prio_ns[1]_ew[0]</t>
-  </si>
-  <si>
-    <t>xp_prio_ns[0]_ew[0]</t>
-  </si>
-  <si>
     <t>xp_bus[3]</t>
   </si>
   <si>
@@ -281,18 +245,6 @@
     <t>xpoint_7_en</t>
   </si>
   <si>
-    <t>xp_bus[0]_prio[1]</t>
-  </si>
-  <si>
-    <t>xp_bus[2]_prio[1]</t>
-  </si>
-  <si>
-    <t>xp_bus[1]_prio[0]</t>
-  </si>
-  <si>
-    <t>xp_bus[3]_prio[0]</t>
-  </si>
-  <si>
     <t>CLB</t>
   </si>
   <si>
@@ -434,12 +386,6 @@
     <t>en_cout</t>
   </si>
   <si>
-    <t>enables cout from LUT on priority[0] as cin for other adders</t>
-  </si>
-  <si>
-    <t>enables cin sourcing from priority[1] for own adder</t>
-  </si>
-  <si>
     <t>presel_0[0]</t>
   </si>
   <si>
@@ -609,6 +555,24 @@
   </si>
   <si>
     <t>en_ce</t>
+  </si>
+  <si>
+    <t>xp_bus[3]_vert[4]</t>
+  </si>
+  <si>
+    <t>xp_bus[2]_vert[5]</t>
+  </si>
+  <si>
+    <t>xp_bus[1]_vert[4]</t>
+  </si>
+  <si>
+    <t>xp_bus[0]_vert[5]</t>
+  </si>
+  <si>
+    <t>enables cin sourcing from bus[5] for own adder</t>
+  </si>
+  <si>
+    <t>enables cout from LUT on bus[4] as cin for other adders</t>
   </si>
 </sst>
 </file>
@@ -1004,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC18F46-B9E9-4D36-8A8B-C506C3DCD618}">
   <dimension ref="A1:H139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="F93" sqref="F93"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="G102" sqref="G102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1027,22 +991,22 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -1054,13 +1018,13 @@
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>84</v>
+        <v>173</v>
       </c>
       <c r="G4" s="2"/>
     </row>
@@ -1073,13 +1037,13 @@
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>82</v>
+        <v>174</v>
       </c>
       <c r="G5" s="2"/>
     </row>
@@ -1092,13 +1056,13 @@
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>83</v>
+        <v>175</v>
       </c>
       <c r="G6" s="2"/>
     </row>
@@ -1111,13 +1075,13 @@
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>81</v>
+        <v>176</v>
       </c>
       <c r="G7" s="2"/>
     </row>
@@ -1130,13 +1094,13 @@
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="G8" s="2"/>
     </row>
@@ -1149,13 +1113,13 @@
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="G9" s="2"/>
     </row>
@@ -1168,13 +1132,13 @@
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="G10" s="2"/>
     </row>
@@ -1187,13 +1151,13 @@
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="G11" s="2"/>
     </row>
@@ -1206,16 +1170,16 @@
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -1227,16 +1191,16 @@
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -1248,16 +1212,16 @@
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -1269,16 +1233,16 @@
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -1290,16 +1254,16 @@
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -1311,16 +1275,16 @@
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -1332,16 +1296,16 @@
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -1353,16 +1317,16 @@
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -1374,12 +1338,12 @@
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="2" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -1391,12 +1355,12 @@
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="2" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -1408,12 +1372,12 @@
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="2" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -1425,12 +1389,12 @@
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="2" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
@@ -1442,12 +1406,12 @@
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="2" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -1459,12 +1423,12 @@
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="2" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
@@ -1476,12 +1440,12 @@
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="2" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
@@ -1493,14 +1457,14 @@
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
@@ -1512,12 +1476,12 @@
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="2" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
@@ -1529,12 +1493,12 @@
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="2" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
@@ -1546,12 +1510,12 @@
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="2" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
@@ -1563,12 +1527,12 @@
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="2" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
@@ -1580,12 +1544,12 @@
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="2" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
@@ -1597,12 +1561,12 @@
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
       <c r="G33" s="2" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
@@ -1614,12 +1578,12 @@
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="G34" s="2" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
@@ -1631,14 +1595,14 @@
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
@@ -1650,12 +1614,12 @@
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
       <c r="G36" s="2" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
@@ -1667,12 +1631,12 @@
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
       <c r="G37" s="2" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
@@ -1684,12 +1648,12 @@
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
       <c r="G38" s="2" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
@@ -1701,12 +1665,12 @@
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
       <c r="G39" s="2" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
@@ -1718,12 +1682,12 @@
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
       <c r="G40" s="2" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
@@ -1735,12 +1699,12 @@
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
       <c r="G41" s="2" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
@@ -1752,12 +1716,12 @@
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
       <c r="G42" s="2" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
@@ -1769,14 +1733,14 @@
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E43" s="5"/>
       <c r="F43" s="5" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
@@ -1788,12 +1752,12 @@
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
       <c r="G44" s="2" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
@@ -1805,12 +1769,12 @@
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
       <c r="G45" s="2" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
@@ -1822,12 +1786,12 @@
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
       <c r="G46" s="2" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
@@ -1839,12 +1803,12 @@
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
       <c r="G47" s="2" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
@@ -1856,12 +1820,12 @@
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
       <c r="G48" s="2" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
@@ -1873,12 +1837,12 @@
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
       <c r="G49" s="2" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
@@ -1890,12 +1854,12 @@
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
       <c r="G50" s="2" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
@@ -1907,14 +1871,14 @@
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E51" s="5"/>
       <c r="F51" s="5" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
@@ -1926,12 +1890,12 @@
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
       <c r="G52" s="2" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
@@ -1943,12 +1907,12 @@
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
       <c r="G53" s="2" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
@@ -1960,12 +1924,12 @@
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
       <c r="G54" s="2" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
@@ -1977,12 +1941,12 @@
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
       <c r="G55" s="2" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
@@ -1994,12 +1958,12 @@
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
       <c r="G56" s="2" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
@@ -2011,12 +1975,12 @@
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
       <c r="G57" s="2" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
@@ -2028,12 +1992,12 @@
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
       <c r="G58" s="2" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
@@ -2045,14 +2009,14 @@
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E59" s="5"/>
       <c r="F59" s="5" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
@@ -2064,12 +2028,12 @@
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
       <c r="G60" s="2" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
@@ -2081,12 +2045,12 @@
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E61" s="5"/>
       <c r="F61" s="5"/>
       <c r="G61" s="2" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
@@ -2098,12 +2062,12 @@
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
       <c r="G62" s="2" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
@@ -2115,12 +2079,12 @@
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E63" s="5"/>
       <c r="F63" s="5"/>
       <c r="G63" s="2" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
@@ -2132,12 +2096,12 @@
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E64" s="5"/>
       <c r="F64" s="5"/>
       <c r="G64" s="2" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
@@ -2149,12 +2113,12 @@
       </c>
       <c r="C65" s="1"/>
       <c r="D65" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
       <c r="G65" s="2" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
@@ -2166,12 +2130,12 @@
       </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E66" s="5"/>
       <c r="F66" s="5"/>
       <c r="G66" s="2" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
@@ -2183,14 +2147,14 @@
       </c>
       <c r="C67" s="1"/>
       <c r="D67" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E67" s="5"/>
       <c r="F67" s="5" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
@@ -2202,12 +2166,12 @@
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E68" s="5"/>
       <c r="F68" s="5"/>
       <c r="G68" s="2" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
@@ -2219,12 +2183,12 @@
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E69" s="5"/>
       <c r="F69" s="5"/>
       <c r="G69" s="2" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
@@ -2236,12 +2200,12 @@
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
       <c r="G70" s="2" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
@@ -2253,12 +2217,12 @@
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>
       <c r="G71" s="2" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.35">
@@ -2270,12 +2234,12 @@
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E72" s="5"/>
       <c r="F72" s="5"/>
       <c r="G72" s="2" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.35">
@@ -2287,12 +2251,12 @@
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
       <c r="G73" s="2" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
@@ -2304,12 +2268,12 @@
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E74" s="5"/>
       <c r="F74" s="5"/>
       <c r="G74" s="2" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.35">
@@ -2321,14 +2285,14 @@
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E75" s="5"/>
       <c r="F75" s="5" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.35">
@@ -2340,12 +2304,12 @@
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E76" s="5"/>
       <c r="F76" s="5"/>
       <c r="G76" s="2" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.35">
@@ -2357,12 +2321,12 @@
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E77" s="5"/>
       <c r="F77" s="5"/>
       <c r="G77" s="2" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.35">
@@ -2374,12 +2338,12 @@
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E78" s="5"/>
       <c r="F78" s="5"/>
       <c r="G78" s="2" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.35">
@@ -2391,12 +2355,12 @@
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E79" s="5"/>
       <c r="F79" s="5"/>
       <c r="G79" s="2" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.35">
@@ -2408,12 +2372,12 @@
       </c>
       <c r="C80" s="1"/>
       <c r="D80" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E80" s="5"/>
       <c r="F80" s="5"/>
       <c r="G80" s="2" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.35">
@@ -2425,12 +2389,12 @@
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E81" s="5"/>
       <c r="F81" s="5"/>
       <c r="G81" s="2" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.35">
@@ -2442,12 +2406,12 @@
       </c>
       <c r="C82" s="1"/>
       <c r="D82" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E82" s="5"/>
       <c r="F82" s="5"/>
       <c r="G82" s="2" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
@@ -2459,14 +2423,14 @@
       </c>
       <c r="C83" s="1"/>
       <c r="D83" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E83" s="5"/>
       <c r="F83" s="5" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.35">
@@ -2478,13 +2442,13 @@
       </c>
       <c r="C84" s="1"/>
       <c r="D84" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="G84" s="2"/>
     </row>
@@ -2497,13 +2461,13 @@
       </c>
       <c r="C85" s="1"/>
       <c r="D85" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="G85" s="2"/>
     </row>
@@ -2516,13 +2480,13 @@
       </c>
       <c r="C86" s="1"/>
       <c r="D86" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="G86" s="2"/>
     </row>
@@ -2535,13 +2499,13 @@
       </c>
       <c r="C87" s="1"/>
       <c r="D87" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="G87" s="2"/>
     </row>
@@ -2554,13 +2518,13 @@
       </c>
       <c r="C88" s="1"/>
       <c r="D88" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F88" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="E88" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="F88" s="5" t="s">
-        <v>101</v>
       </c>
       <c r="G88" s="2"/>
     </row>
@@ -2573,13 +2537,13 @@
       </c>
       <c r="C89" s="1"/>
       <c r="D89" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F89" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F89" s="5" t="s">
-        <v>101</v>
       </c>
       <c r="G89" s="2"/>
     </row>
@@ -2592,13 +2556,13 @@
       </c>
       <c r="C90" s="1"/>
       <c r="D90" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="G90" s="2"/>
     </row>
@@ -2611,13 +2575,13 @@
       </c>
       <c r="C91" s="1"/>
       <c r="D91" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="G91" s="2"/>
     </row>
@@ -2630,16 +2594,16 @@
       </c>
       <c r="C92" s="1"/>
       <c r="D92" s="1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.35">
@@ -2651,13 +2615,13 @@
       </c>
       <c r="C93" s="1"/>
       <c r="D93" s="1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="G93" s="2"/>
     </row>
@@ -2670,13 +2634,13 @@
       </c>
       <c r="C94" s="1"/>
       <c r="D94" s="1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="G94" s="2"/>
     </row>
@@ -2689,13 +2653,13 @@
       </c>
       <c r="C95" s="1"/>
       <c r="D95" s="1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E95" s="5" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="F95" s="5" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="G95" s="2"/>
     </row>
@@ -2708,16 +2672,16 @@
       </c>
       <c r="C96" s="1"/>
       <c r="D96" s="1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>133</v>
+        <v>177</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.35">
@@ -2729,13 +2693,13 @@
       </c>
       <c r="C97" s="1"/>
       <c r="D97" s="1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E97" s="5" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="F97" s="5" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="G97" s="2"/>
     </row>
@@ -2748,13 +2712,13 @@
       </c>
       <c r="C98" s="1"/>
       <c r="D98" s="1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="F98" s="5" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="G98" s="2"/>
     </row>
@@ -2767,13 +2731,13 @@
       </c>
       <c r="C99" s="1"/>
       <c r="D99" s="1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="F99" s="5" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="G99" s="2"/>
     </row>
@@ -2786,16 +2750,16 @@
       </c>
       <c r="C100" s="1"/>
       <c r="D100" s="1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="F100" s="5" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.35">
@@ -2807,13 +2771,13 @@
       </c>
       <c r="C101" s="1"/>
       <c r="D101" s="1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="F101" s="5" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="G101" s="2"/>
     </row>
@@ -2826,13 +2790,13 @@
       </c>
       <c r="C102" s="1"/>
       <c r="D102" s="1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="F102" s="5" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="G102" s="2"/>
     </row>
@@ -2845,13 +2809,13 @@
       </c>
       <c r="C103" s="1"/>
       <c r="D103" s="1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E103" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F103" s="5" t="s">
         <v>119</v>
-      </c>
-      <c r="F103" s="5" t="s">
-        <v>137</v>
       </c>
       <c r="G103" s="2"/>
     </row>
@@ -2864,16 +2828,16 @@
       </c>
       <c r="C104" s="1"/>
       <c r="D104" s="1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="F104" s="5" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="G104" s="2" t="s">
-        <v>132</v>
+        <v>178</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.35">
@@ -2885,13 +2849,13 @@
       </c>
       <c r="C105" s="1"/>
       <c r="D105" s="1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="F105" s="5" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="G105" s="2"/>
     </row>
@@ -2904,13 +2868,13 @@
       </c>
       <c r="C106" s="1"/>
       <c r="D106" s="1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="F106" s="5" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="G106" s="2"/>
     </row>
@@ -2923,13 +2887,13 @@
       </c>
       <c r="C107" s="1"/>
       <c r="D107" s="1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="F107" s="5" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="G107" s="2"/>
     </row>
@@ -2947,11 +2911,11 @@
       <c r="E108" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F108" s="5" t="s">
-        <v>60</v>
+      <c r="F108" s="7" t="s">
+        <v>156</v>
       </c>
       <c r="G108" s="7" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.35">
@@ -2968,11 +2932,11 @@
       <c r="E109" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F109" s="5" t="s">
-        <v>61</v>
+      <c r="F109" s="7" t="s">
+        <v>157</v>
       </c>
       <c r="G109" s="7" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.35">
@@ -2989,11 +2953,11 @@
       <c r="E110" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F110" s="5" t="s">
-        <v>62</v>
+      <c r="F110" s="7" t="s">
+        <v>158</v>
       </c>
       <c r="G110" s="7" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.35">
@@ -3010,11 +2974,11 @@
       <c r="E111" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F111" s="5" t="s">
-        <v>63</v>
+      <c r="F111" s="7" t="s">
+        <v>159</v>
       </c>
       <c r="G111" s="7" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.35">
@@ -3032,10 +2996,10 @@
         <v>7</v>
       </c>
       <c r="F112" s="5" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="G112" s="5" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.35">
@@ -3053,10 +3017,10 @@
         <v>8</v>
       </c>
       <c r="F113" s="5" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="G113" s="5" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.35">
@@ -3074,10 +3038,10 @@
         <v>9</v>
       </c>
       <c r="F114" s="5" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="G114" s="5" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.35">
@@ -3095,10 +3059,10 @@
         <v>10</v>
       </c>
       <c r="F115" s="5" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="G115" s="5" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.35">
@@ -3116,10 +3080,10 @@
         <v>11</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="G116" s="5" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.35">
@@ -3137,10 +3101,10 @@
         <v>12</v>
       </c>
       <c r="F117" s="5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="G117" s="5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.35">
@@ -3158,10 +3122,10 @@
         <v>13</v>
       </c>
       <c r="F118" s="5" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="G118" s="5" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.35">
@@ -3179,10 +3143,10 @@
         <v>14</v>
       </c>
       <c r="F119" s="5" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="G119" s="5" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.35">
@@ -3200,10 +3164,10 @@
         <v>15</v>
       </c>
       <c r="F120" s="5" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="G120" s="5" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.35">
@@ -3221,10 +3185,10 @@
         <v>16</v>
       </c>
       <c r="F121" s="5" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="G121" s="5" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.35">
@@ -3242,10 +3206,10 @@
         <v>17</v>
       </c>
       <c r="F122" s="5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="G122" s="5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.35">
@@ -3263,10 +3227,10 @@
         <v>18</v>
       </c>
       <c r="F123" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G123" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.35">
@@ -3284,10 +3248,10 @@
         <v>19</v>
       </c>
       <c r="F124" s="5" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G124" s="5" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.35">
@@ -3305,10 +3269,10 @@
         <v>20</v>
       </c>
       <c r="F125" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="G125" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.35">
@@ -3326,10 +3290,10 @@
         <v>21</v>
       </c>
       <c r="F126" s="5" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="G126" s="5" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.35">
@@ -3347,10 +3311,10 @@
         <v>22</v>
       </c>
       <c r="F127" s="5" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G127" s="5" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.35">
@@ -3368,10 +3332,10 @@
         <v>23</v>
       </c>
       <c r="F128" s="5" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G128" s="5" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.35">
@@ -3389,10 +3353,10 @@
         <v>24</v>
       </c>
       <c r="F129" s="5" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G129" s="5" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.35">
@@ -3410,10 +3374,10 @@
         <v>25</v>
       </c>
       <c r="F130" s="5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G130" s="5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.35">
@@ -3431,10 +3395,10 @@
         <v>26</v>
       </c>
       <c r="F131" s="5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G131" s="5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.35">
@@ -3452,10 +3416,10 @@
         <v>27</v>
       </c>
       <c r="F132" s="5" t="s">
-        <v>36</v>
+        <v>160</v>
       </c>
       <c r="G132" s="5" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.35">
@@ -3473,10 +3437,10 @@
         <v>28</v>
       </c>
       <c r="F133" s="5" t="s">
-        <v>37</v>
+        <v>161</v>
       </c>
       <c r="G133" s="5" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.35">
@@ -3494,10 +3458,10 @@
         <v>29</v>
       </c>
       <c r="F134" s="5" t="s">
-        <v>38</v>
+        <v>162</v>
       </c>
       <c r="G134" s="5" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.35">
@@ -3515,10 +3479,10 @@
         <v>30</v>
       </c>
       <c r="F135" s="5" t="s">
-        <v>39</v>
+        <v>163</v>
       </c>
       <c r="G135" s="5" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.35">
@@ -3536,10 +3500,10 @@
         <v>31</v>
       </c>
       <c r="F136" s="5" t="s">
-        <v>40</v>
+        <v>164</v>
       </c>
       <c r="G136" s="5" t="s">
-        <v>182</v>
+        <v>164</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.35">
@@ -3557,10 +3521,10 @@
         <v>32</v>
       </c>
       <c r="F137" s="5" t="s">
-        <v>41</v>
+        <v>165</v>
       </c>
       <c r="G137" s="5" t="s">
-        <v>183</v>
+        <v>165</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.35">
@@ -3578,10 +3542,10 @@
         <v>33</v>
       </c>
       <c r="F138" s="5" t="s">
-        <v>42</v>
+        <v>166</v>
       </c>
       <c r="G138" s="5" t="s">
-        <v>184</v>
+        <v>166</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.35">
@@ -3599,10 +3563,10 @@
         <v>34</v>
       </c>
       <c r="F139" s="5" t="s">
-        <v>43</v>
+        <v>167</v>
       </c>
       <c r="G139" s="5" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
built a working "compiler" in C for Arduino
</commit_message>
<xml_diff>
--- a/doc/bitstream_doc.xlsx
+++ b/doc/bitstream_doc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Downloads\FPGA\my-discrete-fpga\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D319443A-5EB1-4F2E-B9F5-BE8771DA5611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC239C9D-17F7-4789-B33C-A041204690C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13260" yWindow="0" windowWidth="12340" windowHeight="14400" xr2:uid="{C7546AD3-8A64-4A61-AF3E-FA211CF4A71C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{C7546AD3-8A64-4A61-AF3E-FA211CF4A71C}"/>
   </bookViews>
   <sheets>
     <sheet name="bitstream" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="183">
   <si>
     <t>Bitstream Documentation for one full slice</t>
   </si>
@@ -573,6 +573,18 @@
   </si>
   <si>
     <t>enables cout from LUT on bus[4] as cin for other adders</t>
+  </si>
+  <si>
+    <t>In Compiler</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>xp_bus[4]</t>
+  </si>
+  <si>
+    <t>xp_bus[5]</t>
   </si>
 </sst>
 </file>
@@ -635,7 +647,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -651,6 +663,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -966,27 +981,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC18F46-B9E9-4D36-8A8B-C506C3DCD618}">
-  <dimension ref="A1:H139"/>
+  <dimension ref="A1:I139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="G102" sqref="G102"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="9.1796875" style="1"/>
-    <col min="5" max="5" width="15.1796875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.1796875" customWidth="1"/>
-    <col min="7" max="7" width="25.81640625" customWidth="1"/>
-    <col min="8" max="8" width="59.54296875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="15.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="25.85546875" customWidth="1"/>
+    <col min="9" max="9" width="59.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" s="4" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -1006,10 +1022,13 @@
         <v>59</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>0</v>
       </c>
@@ -1026,9 +1045,12 @@
       <c r="F4" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G4" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -1045,9 +1067,12 @@
       <c r="F5" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G5" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -1064,9 +1089,12 @@
       <c r="F6" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G6" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -1083,9 +1111,12 @@
       <c r="F7" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G7" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>4</v>
       </c>
@@ -1102,9 +1133,12 @@
       <c r="F8" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G8" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>5</v>
       </c>
@@ -1121,9 +1155,12 @@
       <c r="F9" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G9" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>6</v>
       </c>
@@ -1140,9 +1177,12 @@
       <c r="F10" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G10" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>7</v>
       </c>
@@ -1159,9 +1199,12 @@
       <c r="F11" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G11" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>8</v>
       </c>
@@ -1178,11 +1221,12 @@
       <c r="F12" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="8"/>
+      <c r="H12" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>9</v>
       </c>
@@ -1199,11 +1243,12 @@
       <c r="F13" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="8"/>
+      <c r="H13" s="5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>10</v>
       </c>
@@ -1220,11 +1265,12 @@
       <c r="F14" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="8"/>
+      <c r="H14" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>11</v>
       </c>
@@ -1241,11 +1287,14 @@
       <c r="F15" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>12</v>
       </c>
@@ -1262,11 +1311,14 @@
       <c r="F16" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>13</v>
       </c>
@@ -1283,11 +1335,14 @@
       <c r="F17" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>14</v>
       </c>
@@ -1304,11 +1359,14 @@
       <c r="F18" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>15</v>
       </c>
@@ -1325,11 +1383,14 @@
       <c r="F19" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>16</v>
       </c>
@@ -1342,11 +1403,12 @@
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="5"/>
+      <c r="H20" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>17</v>
       </c>
@@ -1359,11 +1421,12 @@
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="5"/>
+      <c r="H21" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>18</v>
       </c>
@@ -1376,11 +1439,12 @@
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="5"/>
+      <c r="H22" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>19</v>
       </c>
@@ -1393,11 +1457,12 @@
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="5"/>
+      <c r="H23" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>20</v>
       </c>
@@ -1410,11 +1475,12 @@
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="5"/>
+      <c r="H24" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>21</v>
       </c>
@@ -1427,11 +1493,12 @@
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
-      <c r="G25" s="2" t="s">
+      <c r="G25" s="5"/>
+      <c r="H25" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>22</v>
       </c>
@@ -1444,11 +1511,12 @@
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="5"/>
+      <c r="H26" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>23</v>
       </c>
@@ -1463,11 +1531,12 @@
       <c r="F27" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G27" s="5"/>
+      <c r="H27" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>24</v>
       </c>
@@ -1480,11 +1549,12 @@
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
-      <c r="G28" s="2" t="s">
+      <c r="G28" s="5"/>
+      <c r="H28" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>25</v>
       </c>
@@ -1497,11 +1567,12 @@
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
-      <c r="G29" s="2" t="s">
+      <c r="G29" s="5"/>
+      <c r="H29" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>26</v>
       </c>
@@ -1514,11 +1585,12 @@
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
-      <c r="G30" s="2" t="s">
+      <c r="G30" s="5"/>
+      <c r="H30" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>27</v>
       </c>
@@ -1531,11 +1603,12 @@
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
-      <c r="G31" s="2" t="s">
+      <c r="G31" s="5"/>
+      <c r="H31" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>28</v>
       </c>
@@ -1548,11 +1621,12 @@
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
-      <c r="G32" s="2" t="s">
+      <c r="G32" s="5"/>
+      <c r="H32" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>29</v>
       </c>
@@ -1565,11 +1639,12 @@
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
-      <c r="G33" s="2" t="s">
+      <c r="G33" s="5"/>
+      <c r="H33" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>30</v>
       </c>
@@ -1582,11 +1657,12 @@
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
-      <c r="G34" s="2" t="s">
+      <c r="G34" s="5"/>
+      <c r="H34" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>31</v>
       </c>
@@ -1601,11 +1677,12 @@
       <c r="F35" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="G35" s="5"/>
+      <c r="H35" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>32</v>
       </c>
@@ -1618,11 +1695,12 @@
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
-      <c r="G36" s="2" t="s">
+      <c r="G36" s="5"/>
+      <c r="H36" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>33</v>
       </c>
@@ -1635,11 +1713,12 @@
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
-      <c r="G37" s="2" t="s">
+      <c r="G37" s="5"/>
+      <c r="H37" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>34</v>
       </c>
@@ -1652,11 +1731,12 @@
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
-      <c r="G38" s="2" t="s">
+      <c r="G38" s="5"/>
+      <c r="H38" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>35</v>
       </c>
@@ -1669,11 +1749,12 @@
       </c>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
-      <c r="G39" s="2" t="s">
+      <c r="G39" s="5"/>
+      <c r="H39" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>36</v>
       </c>
@@ -1686,11 +1767,12 @@
       </c>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
-      <c r="G40" s="2" t="s">
+      <c r="G40" s="5"/>
+      <c r="H40" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>37</v>
       </c>
@@ -1703,11 +1785,12 @@
       </c>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
-      <c r="G41" s="2" t="s">
+      <c r="G41" s="5"/>
+      <c r="H41" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>38</v>
       </c>
@@ -1720,11 +1803,12 @@
       </c>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
-      <c r="G42" s="2" t="s">
+      <c r="G42" s="5"/>
+      <c r="H42" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>39</v>
       </c>
@@ -1739,11 +1823,12 @@
       <c r="F43" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="G43" s="5"/>
+      <c r="H43" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>40</v>
       </c>
@@ -1756,11 +1841,12 @@
       </c>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
-      <c r="G44" s="2" t="s">
+      <c r="G44" s="5"/>
+      <c r="H44" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>41</v>
       </c>
@@ -1773,11 +1859,12 @@
       </c>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
-      <c r="G45" s="2" t="s">
+      <c r="G45" s="5"/>
+      <c r="H45" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>42</v>
       </c>
@@ -1790,11 +1877,12 @@
       </c>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
-      <c r="G46" s="2" t="s">
+      <c r="G46" s="5"/>
+      <c r="H46" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>43</v>
       </c>
@@ -1807,11 +1895,12 @@
       </c>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
-      <c r="G47" s="2" t="s">
+      <c r="G47" s="5"/>
+      <c r="H47" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>44</v>
       </c>
@@ -1824,11 +1913,12 @@
       </c>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
-      <c r="G48" s="2" t="s">
+      <c r="G48" s="5"/>
+      <c r="H48" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>45</v>
       </c>
@@ -1841,11 +1931,12 @@
       </c>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
-      <c r="G49" s="2" t="s">
+      <c r="G49" s="5"/>
+      <c r="H49" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>46</v>
       </c>
@@ -1858,11 +1949,12 @@
       </c>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
-      <c r="G50" s="2" t="s">
+      <c r="G50" s="5"/>
+      <c r="H50" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>47</v>
       </c>
@@ -1877,11 +1969,12 @@
       <c r="F51" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="G51" s="2" t="s">
+      <c r="G51" s="5"/>
+      <c r="H51" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>48</v>
       </c>
@@ -1894,11 +1987,12 @@
       </c>
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
-      <c r="G52" s="2" t="s">
+      <c r="G52" s="5"/>
+      <c r="H52" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>49</v>
       </c>
@@ -1911,11 +2005,12 @@
       </c>
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
-      <c r="G53" s="2" t="s">
+      <c r="G53" s="5"/>
+      <c r="H53" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>50</v>
       </c>
@@ -1928,11 +2023,12 @@
       </c>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
-      <c r="G54" s="2" t="s">
+      <c r="G54" s="5"/>
+      <c r="H54" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>51</v>
       </c>
@@ -1945,11 +2041,12 @@
       </c>
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
-      <c r="G55" s="2" t="s">
+      <c r="G55" s="5"/>
+      <c r="H55" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>52</v>
       </c>
@@ -1962,11 +2059,12 @@
       </c>
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
-      <c r="G56" s="2" t="s">
+      <c r="G56" s="5"/>
+      <c r="H56" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>53</v>
       </c>
@@ -1979,11 +2077,12 @@
       </c>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
-      <c r="G57" s="2" t="s">
+      <c r="G57" s="5"/>
+      <c r="H57" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>54</v>
       </c>
@@ -1996,11 +2095,12 @@
       </c>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
-      <c r="G58" s="2" t="s">
+      <c r="G58" s="5"/>
+      <c r="H58" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>55</v>
       </c>
@@ -2015,11 +2115,12 @@
       <c r="F59" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="G59" s="2" t="s">
+      <c r="G59" s="5"/>
+      <c r="H59" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>56</v>
       </c>
@@ -2032,11 +2133,12 @@
       </c>
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
-      <c r="G60" s="2" t="s">
+      <c r="G60" s="5"/>
+      <c r="H60" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>57</v>
       </c>
@@ -2049,11 +2151,12 @@
       </c>
       <c r="E61" s="5"/>
       <c r="F61" s="5"/>
-      <c r="G61" s="2" t="s">
+      <c r="G61" s="5"/>
+      <c r="H61" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>58</v>
       </c>
@@ -2066,11 +2169,12 @@
       </c>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
-      <c r="G62" s="2" t="s">
+      <c r="G62" s="5"/>
+      <c r="H62" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>59</v>
       </c>
@@ -2083,11 +2187,12 @@
       </c>
       <c r="E63" s="5"/>
       <c r="F63" s="5"/>
-      <c r="G63" s="2" t="s">
+      <c r="G63" s="5"/>
+      <c r="H63" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>60</v>
       </c>
@@ -2100,11 +2205,12 @@
       </c>
       <c r="E64" s="5"/>
       <c r="F64" s="5"/>
-      <c r="G64" s="2" t="s">
+      <c r="G64" s="5"/>
+      <c r="H64" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>61</v>
       </c>
@@ -2117,11 +2223,12 @@
       </c>
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
-      <c r="G65" s="2" t="s">
+      <c r="G65" s="5"/>
+      <c r="H65" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>62</v>
       </c>
@@ -2134,11 +2241,12 @@
       </c>
       <c r="E66" s="5"/>
       <c r="F66" s="5"/>
-      <c r="G66" s="2" t="s">
+      <c r="G66" s="5"/>
+      <c r="H66" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>63</v>
       </c>
@@ -2153,11 +2261,12 @@
       <c r="F67" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="G67" s="2" t="s">
+      <c r="G67" s="5"/>
+      <c r="H67" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>64</v>
       </c>
@@ -2170,11 +2279,12 @@
       </c>
       <c r="E68" s="5"/>
       <c r="F68" s="5"/>
-      <c r="G68" s="2" t="s">
+      <c r="G68" s="5"/>
+      <c r="H68" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>65</v>
       </c>
@@ -2187,11 +2297,12 @@
       </c>
       <c r="E69" s="5"/>
       <c r="F69" s="5"/>
-      <c r="G69" s="2" t="s">
+      <c r="G69" s="5"/>
+      <c r="H69" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>66</v>
       </c>
@@ -2204,11 +2315,12 @@
       </c>
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
-      <c r="G70" s="2" t="s">
+      <c r="G70" s="5"/>
+      <c r="H70" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>67</v>
       </c>
@@ -2221,11 +2333,12 @@
       </c>
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>
-      <c r="G71" s="2" t="s">
+      <c r="G71" s="5"/>
+      <c r="H71" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>68</v>
       </c>
@@ -2238,11 +2351,12 @@
       </c>
       <c r="E72" s="5"/>
       <c r="F72" s="5"/>
-      <c r="G72" s="2" t="s">
+      <c r="G72" s="5"/>
+      <c r="H72" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>69</v>
       </c>
@@ -2255,11 +2369,12 @@
       </c>
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
-      <c r="G73" s="2" t="s">
+      <c r="G73" s="5"/>
+      <c r="H73" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>70</v>
       </c>
@@ -2272,11 +2387,12 @@
       </c>
       <c r="E74" s="5"/>
       <c r="F74" s="5"/>
-      <c r="G74" s="2" t="s">
+      <c r="G74" s="5"/>
+      <c r="H74" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>71</v>
       </c>
@@ -2291,11 +2407,12 @@
       <c r="F75" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="G75" s="2" t="s">
+      <c r="G75" s="5"/>
+      <c r="H75" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>72</v>
       </c>
@@ -2308,11 +2425,12 @@
       </c>
       <c r="E76" s="5"/>
       <c r="F76" s="5"/>
-      <c r="G76" s="2" t="s">
+      <c r="G76" s="5"/>
+      <c r="H76" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>73</v>
       </c>
@@ -2325,11 +2443,12 @@
       </c>
       <c r="E77" s="5"/>
       <c r="F77" s="5"/>
-      <c r="G77" s="2" t="s">
+      <c r="G77" s="5"/>
+      <c r="H77" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>74</v>
       </c>
@@ -2342,11 +2461,12 @@
       </c>
       <c r="E78" s="5"/>
       <c r="F78" s="5"/>
-      <c r="G78" s="2" t="s">
+      <c r="G78" s="5"/>
+      <c r="H78" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>75</v>
       </c>
@@ -2359,11 +2479,12 @@
       </c>
       <c r="E79" s="5"/>
       <c r="F79" s="5"/>
-      <c r="G79" s="2" t="s">
+      <c r="G79" s="5"/>
+      <c r="H79" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>76</v>
       </c>
@@ -2376,11 +2497,12 @@
       </c>
       <c r="E80" s="5"/>
       <c r="F80" s="5"/>
-      <c r="G80" s="2" t="s">
+      <c r="G80" s="5"/>
+      <c r="H80" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>77</v>
       </c>
@@ -2393,11 +2515,12 @@
       </c>
       <c r="E81" s="5"/>
       <c r="F81" s="5"/>
-      <c r="G81" s="2" t="s">
+      <c r="G81" s="5"/>
+      <c r="H81" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>78</v>
       </c>
@@ -2410,11 +2533,12 @@
       </c>
       <c r="E82" s="5"/>
       <c r="F82" s="5"/>
-      <c r="G82" s="2" t="s">
+      <c r="G82" s="5"/>
+      <c r="H82" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>79</v>
       </c>
@@ -2429,11 +2553,12 @@
       <c r="F83" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="G83" s="2" t="s">
+      <c r="G83" s="5"/>
+      <c r="H83" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>80</v>
       </c>
@@ -2450,9 +2575,10 @@
       <c r="F84" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G84" s="2"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G84" s="5"/>
+      <c r="H84" s="2"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>81</v>
       </c>
@@ -2469,9 +2595,10 @@
       <c r="F85" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G85" s="2"/>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G85" s="5"/>
+      <c r="H85" s="2"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>82</v>
       </c>
@@ -2488,9 +2615,10 @@
       <c r="F86" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="G86" s="2"/>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G86" s="5"/>
+      <c r="H86" s="2"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>83</v>
       </c>
@@ -2507,9 +2635,10 @@
       <c r="F87" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="G87" s="2"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G87" s="5"/>
+      <c r="H87" s="2"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>84</v>
       </c>
@@ -2526,9 +2655,10 @@
       <c r="F88" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="G88" s="2"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G88" s="5"/>
+      <c r="H88" s="2"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>85</v>
       </c>
@@ -2545,9 +2675,10 @@
       <c r="F89" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="G89" s="2"/>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G89" s="5"/>
+      <c r="H89" s="2"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>86</v>
       </c>
@@ -2564,9 +2695,10 @@
       <c r="F90" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="G90" s="2"/>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G90" s="5"/>
+      <c r="H90" s="2"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>87</v>
       </c>
@@ -2583,9 +2715,10 @@
       <c r="F91" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="G91" s="2"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G91" s="5"/>
+      <c r="H91" s="2"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>88</v>
       </c>
@@ -2602,11 +2735,12 @@
       <c r="F92" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="G92" s="2" t="s">
+      <c r="G92" s="5"/>
+      <c r="H92" s="2" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>89</v>
       </c>
@@ -2623,9 +2757,10 @@
       <c r="F93" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="G93" s="2"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G93" s="5"/>
+      <c r="H93" s="2"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>90</v>
       </c>
@@ -2642,9 +2777,10 @@
       <c r="F94" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="G94" s="2"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G94" s="5"/>
+      <c r="H94" s="2"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>91</v>
       </c>
@@ -2661,9 +2797,10 @@
       <c r="F95" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="G95" s="2"/>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G95" s="5"/>
+      <c r="H95" s="2"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>92</v>
       </c>
@@ -2680,11 +2817,12 @@
       <c r="F96" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G96" s="2" t="s">
+      <c r="G96" s="5"/>
+      <c r="H96" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>93</v>
       </c>
@@ -2701,9 +2839,10 @@
       <c r="F97" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="G97" s="2"/>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G97" s="5"/>
+      <c r="H97" s="2"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>94</v>
       </c>
@@ -2720,9 +2859,10 @@
       <c r="F98" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="G98" s="2"/>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G98" s="5"/>
+      <c r="H98" s="2"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>95</v>
       </c>
@@ -2739,9 +2879,10 @@
       <c r="F99" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="G99" s="2"/>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G99" s="5"/>
+      <c r="H99" s="2"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>96</v>
       </c>
@@ -2758,11 +2899,12 @@
       <c r="F100" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="G100" s="2" t="s">
+      <c r="G100" s="5"/>
+      <c r="H100" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>97</v>
       </c>
@@ -2779,9 +2921,10 @@
       <c r="F101" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="G101" s="2"/>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G101" s="5"/>
+      <c r="H101" s="2"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>98</v>
       </c>
@@ -2798,9 +2941,10 @@
       <c r="F102" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="G102" s="2"/>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G102" s="5"/>
+      <c r="H102" s="2"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>99</v>
       </c>
@@ -2817,9 +2961,10 @@
       <c r="F103" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="G103" s="2"/>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G103" s="5"/>
+      <c r="H103" s="2"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>100</v>
       </c>
@@ -2836,11 +2981,12 @@
       <c r="F104" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="G104" s="2" t="s">
+      <c r="G104" s="5"/>
+      <c r="H104" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>101</v>
       </c>
@@ -2857,9 +3003,10 @@
       <c r="F105" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="G105" s="2"/>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G105" s="5"/>
+      <c r="H105" s="2"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>102</v>
       </c>
@@ -2876,9 +3023,10 @@
       <c r="F106" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="G106" s="2"/>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G106" s="5"/>
+      <c r="H106" s="2"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>103</v>
       </c>
@@ -2895,9 +3043,10 @@
       <c r="F107" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G107" s="2"/>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G107" s="5"/>
+      <c r="H107" s="2"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>104</v>
       </c>
@@ -2914,11 +3063,14 @@
       <c r="F108" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="G108" s="7" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G108" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H108" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>105</v>
       </c>
@@ -2935,11 +3087,14 @@
       <c r="F109" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="G109" s="7" t="s">
+      <c r="G109" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H109" s="7" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <v>106</v>
       </c>
@@ -2956,11 +3111,14 @@
       <c r="F110" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="G110" s="7" t="s">
+      <c r="G110" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H110" s="7" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>107</v>
       </c>
@@ -2977,11 +3135,14 @@
       <c r="F111" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="G111" s="7" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G111" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H111" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
         <v>108</v>
       </c>
@@ -2998,11 +3159,14 @@
       <c r="F112" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G112" s="5" t="s">
+      <c r="G112" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H112" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
         <v>109</v>
       </c>
@@ -3019,11 +3183,14 @@
       <c r="F113" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G113" s="5" t="s">
+      <c r="G113" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H113" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
         <v>110</v>
       </c>
@@ -3040,11 +3207,14 @@
       <c r="F114" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G114" s="5" t="s">
+      <c r="G114" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H114" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>111</v>
       </c>
@@ -3061,11 +3231,14 @@
       <c r="F115" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G115" s="5" t="s">
+      <c r="G115" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H115" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
         <v>112</v>
       </c>
@@ -3082,11 +3255,14 @@
       <c r="F116" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G116" s="5" t="s">
+      <c r="G116" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H116" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
         <v>113</v>
       </c>
@@ -3103,11 +3279,14 @@
       <c r="F117" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G117" s="5" t="s">
+      <c r="G117" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H117" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
         <v>114</v>
       </c>
@@ -3124,11 +3303,14 @@
       <c r="F118" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G118" s="5" t="s">
+      <c r="G118" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H118" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="3">
         <v>115</v>
       </c>
@@ -3145,11 +3327,14 @@
       <c r="F119" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="G119" s="5" t="s">
+      <c r="G119" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H119" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="3">
         <v>116</v>
       </c>
@@ -3166,11 +3351,14 @@
       <c r="F120" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="G120" s="5" t="s">
+      <c r="G120" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H120" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
         <v>117</v>
       </c>
@@ -3187,11 +3375,14 @@
       <c r="F121" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G121" s="5" t="s">
+      <c r="G121" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H121" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
         <v>118</v>
       </c>
@@ -3208,11 +3399,14 @@
       <c r="F122" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G122" s="5" t="s">
+      <c r="G122" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H122" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="3">
         <v>119</v>
       </c>
@@ -3229,11 +3423,14 @@
       <c r="F123" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G123" s="5" t="s">
+      <c r="G123" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H123" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="3">
         <v>120</v>
       </c>
@@ -3250,11 +3447,14 @@
       <c r="F124" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G124" s="5" t="s">
+      <c r="G124" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H124" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="3">
         <v>121</v>
       </c>
@@ -3271,11 +3471,14 @@
       <c r="F125" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G125" s="5" t="s">
+      <c r="G125" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H125" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="3">
         <v>122</v>
       </c>
@@ -3292,11 +3495,14 @@
       <c r="F126" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G126" s="5" t="s">
+      <c r="G126" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H126" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="3">
         <v>123</v>
       </c>
@@ -3313,11 +3519,14 @@
       <c r="F127" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G127" s="5" t="s">
+      <c r="G127" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H127" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="3">
         <v>124</v>
       </c>
@@ -3334,11 +3543,14 @@
       <c r="F128" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G128" s="5" t="s">
+      <c r="G128" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H128" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="3">
         <v>125</v>
       </c>
@@ -3355,11 +3567,14 @@
       <c r="F129" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G129" s="5" t="s">
+      <c r="G129" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H129" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="3">
         <v>126</v>
       </c>
@@ -3376,11 +3591,14 @@
       <c r="F130" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G130" s="5" t="s">
+      <c r="G130" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H130" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="3">
         <v>127</v>
       </c>
@@ -3397,11 +3615,14 @@
       <c r="F131" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G131" s="5" t="s">
+      <c r="G131" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H131" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="3">
         <v>128</v>
       </c>
@@ -3418,11 +3639,14 @@
       <c r="F132" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="G132" s="5" t="s">
+      <c r="G132" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H132" s="5" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="3">
         <v>129</v>
       </c>
@@ -3439,11 +3663,14 @@
       <c r="F133" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="G133" s="5" t="s">
+      <c r="G133" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H133" s="5" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="3">
         <v>130</v>
       </c>
@@ -3460,11 +3687,14 @@
       <c r="F134" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="G134" s="5" t="s">
+      <c r="G134" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H134" s="5" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="3">
         <v>131</v>
       </c>
@@ -3481,11 +3711,14 @@
       <c r="F135" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="G135" s="5" t="s">
+      <c r="G135" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H135" s="5" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="3">
         <v>132</v>
       </c>
@@ -3502,11 +3735,14 @@
       <c r="F136" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="G136" s="5" t="s">
+      <c r="G136" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H136" s="5" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="3">
         <v>133</v>
       </c>
@@ -3523,11 +3759,14 @@
       <c r="F137" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="G137" s="5" t="s">
+      <c r="G137" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H137" s="5" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="3">
         <v>134</v>
       </c>
@@ -3544,11 +3783,14 @@
       <c r="F138" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="G138" s="5" t="s">
+      <c r="G138" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H138" s="5" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="3">
         <v>135</v>
       </c>
@@ -3565,7 +3807,10 @@
       <c r="F139" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="G139" s="5" t="s">
+      <c r="G139" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H139" s="5" t="s">
         <v>167</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated images for blogpost
</commit_message>
<xml_diff>
--- a/doc/bitstream_doc.xlsx
+++ b/doc/bitstream_doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Downloads\FPGA\my-discrete-fpga\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC239C9D-17F7-4789-B33C-A041204690C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE794AD7-1372-46B8-980E-3A546418AAC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{C7546AD3-8A64-4A61-AF3E-FA211CF4A71C}"/>
+    <workbookView xWindow="10110" yWindow="1790" windowWidth="12960" windowHeight="10170" xr2:uid="{C7546AD3-8A64-4A61-AF3E-FA211CF4A71C}"/>
   </bookViews>
   <sheets>
     <sheet name="bitstream" sheetId="3" r:id="rId1"/>
@@ -575,9 +575,6 @@
     <t>enables cout from LUT on bus[4] as cin for other adders</t>
   </si>
   <si>
-    <t>In Compiler</t>
-  </si>
-  <si>
     <t>OK</t>
   </si>
   <si>
@@ -585,6 +582,9 @@
   </si>
   <si>
     <t>xp_bus[5]</t>
+  </si>
+  <si>
+    <t>Implemented in Compiler</t>
   </si>
 </sst>
 </file>
@@ -983,26 +983,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC18F46-B9E9-4D36-8A8B-C506C3DCD618}">
   <dimension ref="A1:I139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="15.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="25.85546875" customWidth="1"/>
-    <col min="9" max="9" width="59.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" style="1"/>
+    <col min="5" max="5" width="15.1796875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.1796875" customWidth="1"/>
+    <col min="7" max="7" width="12.7265625" customWidth="1"/>
+    <col min="8" max="8" width="25.81640625" customWidth="1"/>
+    <col min="9" max="9" width="59.54296875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="4" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -1022,13 +1022,13 @@
         <v>59</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>0</v>
       </c>
@@ -1046,11 +1046,11 @@
         <v>173</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -1068,11 +1068,11 @@
         <v>174</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -1090,11 +1090,11 @@
         <v>175</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -1112,11 +1112,11 @@
         <v>176</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>4</v>
       </c>
@@ -1134,11 +1134,11 @@
         <v>52</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>5</v>
       </c>
@@ -1156,11 +1156,11 @@
         <v>53</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>6</v>
       </c>
@@ -1178,11 +1178,11 @@
         <v>54</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>7</v>
       </c>
@@ -1200,11 +1200,11 @@
         <v>55</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>8</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>9</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>10</v>
       </c>
@@ -1270,7 +1270,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>11</v>
       </c>
@@ -1288,13 +1288,13 @@
         <v>93</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>12</v>
       </c>
@@ -1312,13 +1312,13 @@
         <v>91</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>13</v>
       </c>
@@ -1336,13 +1336,13 @@
         <v>90</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>14</v>
       </c>
@@ -1360,13 +1360,13 @@
         <v>89</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>15</v>
       </c>
@@ -1384,13 +1384,13 @@
         <v>88</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>16</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>17</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>18</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>19</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>20</v>
       </c>
@@ -1480,7 +1480,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>21</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>22</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>23</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>24</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>25</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>26</v>
       </c>
@@ -1590,7 +1590,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>27</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>28</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>29</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>30</v>
       </c>
@@ -1662,7 +1662,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>31</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>32</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>33</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>34</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>35</v>
       </c>
@@ -1754,7 +1754,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>36</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>37</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>38</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>39</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>40</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>41</v>
       </c>
@@ -1864,7 +1864,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>42</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>43</v>
       </c>
@@ -1900,7 +1900,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>44</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>45</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>46</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>47</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>48</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>49</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>50</v>
       </c>
@@ -2028,7 +2028,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>51</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>52</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
         <v>53</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
         <v>54</v>
       </c>
@@ -2100,7 +2100,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
         <v>55</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" s="3">
         <v>56</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="3">
         <v>57</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="3">
         <v>58</v>
       </c>
@@ -2174,7 +2174,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="3">
         <v>59</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="3">
         <v>60</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
         <v>61</v>
       </c>
@@ -2228,7 +2228,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" s="3">
         <v>62</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" s="3">
         <v>63</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" s="3">
         <v>64</v>
       </c>
@@ -2284,7 +2284,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" s="3">
         <v>65</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" s="3">
         <v>66</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" s="3">
         <v>67</v>
       </c>
@@ -2338,7 +2338,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" s="3">
         <v>68</v>
       </c>
@@ -2356,7 +2356,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" s="3">
         <v>69</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" s="3">
         <v>70</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" s="3">
         <v>71</v>
       </c>
@@ -2412,7 +2412,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" s="3">
         <v>72</v>
       </c>
@@ -2430,7 +2430,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" s="3">
         <v>73</v>
       </c>
@@ -2448,7 +2448,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" s="3">
         <v>74</v>
       </c>
@@ -2466,7 +2466,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" s="3">
         <v>75</v>
       </c>
@@ -2484,7 +2484,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" s="3">
         <v>76</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" s="3">
         <v>77</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" s="3">
         <v>78</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83" s="3">
         <v>79</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" s="3">
         <v>80</v>
       </c>
@@ -2578,7 +2578,7 @@
       <c r="G84" s="5"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" s="3">
         <v>81</v>
       </c>
@@ -2598,7 +2598,7 @@
       <c r="G85" s="5"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" s="3">
         <v>82</v>
       </c>
@@ -2618,7 +2618,7 @@
       <c r="G86" s="5"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" s="3">
         <v>83</v>
       </c>
@@ -2638,7 +2638,7 @@
       <c r="G87" s="5"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" s="3">
         <v>84</v>
       </c>
@@ -2658,7 +2658,7 @@
       <c r="G88" s="5"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" s="3">
         <v>85</v>
       </c>
@@ -2678,7 +2678,7 @@
       <c r="G89" s="5"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" s="3">
         <v>86</v>
       </c>
@@ -2698,7 +2698,7 @@
       <c r="G90" s="5"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" s="3">
         <v>87</v>
       </c>
@@ -2718,7 +2718,7 @@
       <c r="G91" s="5"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" s="3">
         <v>88</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" s="3">
         <v>89</v>
       </c>
@@ -2760,7 +2760,7 @@
       <c r="G93" s="5"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A94" s="3">
         <v>90</v>
       </c>
@@ -2780,7 +2780,7 @@
       <c r="G94" s="5"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95" s="3">
         <v>91</v>
       </c>
@@ -2800,7 +2800,7 @@
       <c r="G95" s="5"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96" s="3">
         <v>92</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" s="3">
         <v>93</v>
       </c>
@@ -2842,7 +2842,7 @@
       <c r="G97" s="5"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" s="3">
         <v>94</v>
       </c>
@@ -2862,7 +2862,7 @@
       <c r="G98" s="5"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" s="3">
         <v>95</v>
       </c>
@@ -2882,7 +2882,7 @@
       <c r="G99" s="5"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" s="3">
         <v>96</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" s="3">
         <v>97</v>
       </c>
@@ -2924,7 +2924,7 @@
       <c r="G101" s="5"/>
       <c r="H101" s="2"/>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" s="3">
         <v>98</v>
       </c>
@@ -2944,7 +2944,7 @@
       <c r="G102" s="5"/>
       <c r="H102" s="2"/>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" s="3">
         <v>99</v>
       </c>
@@ -2964,7 +2964,7 @@
       <c r="G103" s="5"/>
       <c r="H103" s="2"/>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" s="3">
         <v>100</v>
       </c>
@@ -2986,7 +2986,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" s="3">
         <v>101</v>
       </c>
@@ -3006,7 +3006,7 @@
       <c r="G105" s="5"/>
       <c r="H105" s="2"/>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" s="3">
         <v>102</v>
       </c>
@@ -3026,7 +3026,7 @@
       <c r="G106" s="5"/>
       <c r="H106" s="2"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107" s="3">
         <v>103</v>
       </c>
@@ -3046,7 +3046,7 @@
       <c r="G107" s="5"/>
       <c r="H107" s="2"/>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A108" s="3">
         <v>104</v>
       </c>
@@ -3064,13 +3064,13 @@
         <v>156</v>
       </c>
       <c r="G108" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H108" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109" s="3">
         <v>105</v>
       </c>
@@ -3088,13 +3088,13 @@
         <v>157</v>
       </c>
       <c r="G109" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H109" s="7" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A110" s="3">
         <v>106</v>
       </c>
@@ -3112,13 +3112,13 @@
         <v>158</v>
       </c>
       <c r="G110" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H110" s="7" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A111" s="3">
         <v>107</v>
       </c>
@@ -3136,13 +3136,13 @@
         <v>159</v>
       </c>
       <c r="G111" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="H111" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="H111" s="5" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A112" s="3">
         <v>108</v>
       </c>
@@ -3160,13 +3160,13 @@
         <v>52</v>
       </c>
       <c r="G112" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H112" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A113" s="3">
         <v>109</v>
       </c>
@@ -3184,13 +3184,13 @@
         <v>53</v>
       </c>
       <c r="G113" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H113" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A114" s="3">
         <v>110</v>
       </c>
@@ -3208,13 +3208,13 @@
         <v>54</v>
       </c>
       <c r="G114" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H114" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A115" s="3">
         <v>111</v>
       </c>
@@ -3232,13 +3232,13 @@
         <v>55</v>
       </c>
       <c r="G115" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H115" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116" s="3">
         <v>112</v>
       </c>
@@ -3256,13 +3256,13 @@
         <v>44</v>
       </c>
       <c r="G116" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H116" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A117" s="3">
         <v>113</v>
       </c>
@@ -3280,13 +3280,13 @@
         <v>45</v>
       </c>
       <c r="G117" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H117" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A118" s="3">
         <v>114</v>
       </c>
@@ -3304,13 +3304,13 @@
         <v>46</v>
       </c>
       <c r="G118" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H118" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A119" s="3">
         <v>115</v>
       </c>
@@ -3328,13 +3328,13 @@
         <v>47</v>
       </c>
       <c r="G119" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H119" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A120" s="3">
         <v>116</v>
       </c>
@@ -3352,13 +3352,13 @@
         <v>48</v>
       </c>
       <c r="G120" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H120" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A121" s="3">
         <v>117</v>
       </c>
@@ -3376,13 +3376,13 @@
         <v>49</v>
       </c>
       <c r="G121" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H121" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A122" s="3">
         <v>118</v>
       </c>
@@ -3400,13 +3400,13 @@
         <v>50</v>
       </c>
       <c r="G122" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H122" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A123" s="3">
         <v>119</v>
       </c>
@@ -3424,13 +3424,13 @@
         <v>51</v>
       </c>
       <c r="G123" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H123" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A124" s="3">
         <v>120</v>
       </c>
@@ -3448,13 +3448,13 @@
         <v>37</v>
       </c>
       <c r="G124" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H124" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A125" s="3">
         <v>121</v>
       </c>
@@ -3472,13 +3472,13 @@
         <v>38</v>
       </c>
       <c r="G125" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H125" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A126" s="3">
         <v>122</v>
       </c>
@@ -3496,13 +3496,13 @@
         <v>36</v>
       </c>
       <c r="G126" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H126" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A127" s="3">
         <v>123</v>
       </c>
@@ -3520,13 +3520,13 @@
         <v>39</v>
       </c>
       <c r="G127" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H127" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A128" s="3">
         <v>124</v>
       </c>
@@ -3544,13 +3544,13 @@
         <v>40</v>
       </c>
       <c r="G128" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H128" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A129" s="3">
         <v>125</v>
       </c>
@@ -3568,13 +3568,13 @@
         <v>41</v>
       </c>
       <c r="G129" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H129" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A130" s="3">
         <v>126</v>
       </c>
@@ -3592,13 +3592,13 @@
         <v>42</v>
       </c>
       <c r="G130" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H130" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A131" s="3">
         <v>127</v>
       </c>
@@ -3616,13 +3616,13 @@
         <v>43</v>
       </c>
       <c r="G131" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H131" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A132" s="3">
         <v>128</v>
       </c>
@@ -3640,13 +3640,13 @@
         <v>160</v>
       </c>
       <c r="G132" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H132" s="5" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A133" s="3">
         <v>129</v>
       </c>
@@ -3664,13 +3664,13 @@
         <v>161</v>
       </c>
       <c r="G133" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H133" s="5" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A134" s="3">
         <v>130</v>
       </c>
@@ -3688,13 +3688,13 @@
         <v>162</v>
       </c>
       <c r="G134" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H134" s="5" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A135" s="3">
         <v>131</v>
       </c>
@@ -3712,13 +3712,13 @@
         <v>163</v>
       </c>
       <c r="G135" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H135" s="5" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A136" s="3">
         <v>132</v>
       </c>
@@ -3736,13 +3736,13 @@
         <v>164</v>
       </c>
       <c r="G136" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H136" s="5" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A137" s="3">
         <v>133</v>
       </c>
@@ -3760,13 +3760,13 @@
         <v>165</v>
       </c>
       <c r="G137" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H137" s="5" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A138" s="3">
         <v>134</v>
       </c>
@@ -3784,13 +3784,13 @@
         <v>166</v>
       </c>
       <c r="G138" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H138" s="5" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A139" s="3">
         <v>135</v>
       </c>
@@ -3808,7 +3808,7 @@
         <v>167</v>
       </c>
       <c r="G139" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H139" s="5" t="s">
         <v>167</v>

</xml_diff>